<commit_message>
NEES import and transpose
</commit_message>
<xml_diff>
--- a/SourceData/NEES.xlsx
+++ b/SourceData/NEES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DCE646B-6FF0-1F46-99DD-232238E5F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52ED220-89CF-5247-9ACA-5515F324DBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="1160" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
+    <workbookView xWindow="2500" yWindow="1040" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>TMEM214</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>mboat7</t>
+  </si>
+  <si>
+    <t>NEMP1-2</t>
+  </si>
+  <si>
+    <t>WFS1-2</t>
+  </si>
+  <si>
+    <t>mboat7-2</t>
   </si>
 </sst>
 </file>
@@ -527,9 +536,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC4DC55-F2F9-5F4B-B79C-9C9FBA074888}">
-  <dimension ref="A1:AN114"/>
+  <dimension ref="A1:AN113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -583,7 +594,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>16</v>
@@ -592,7 +603,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>18</v>
@@ -628,7 +639,7 @@
         <v>26</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AG1" s="2" t="s">
         <v>27</v>
@@ -656,1135 +667,1105 @@
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>2</v>
-      </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="S2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
-        <v>2</v>
-      </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="2">
-        <v>1</v>
-      </c>
-      <c r="X2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1">
+        <v>0.621</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="O2" s="1">
+        <v>3.6139999999999999</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1.526</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>0.499</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1.2689999999999999</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>0.86499999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <v>0.74199999999999999</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
-        <v>0.47499999999999998</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1">
-        <v>0.621</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="N3" s="1">
-        <v>0.91</v>
+        <v>0.64</v>
       </c>
       <c r="O3" s="1">
-        <v>3.6139999999999999</v>
+        <v>4.2359999999999998</v>
       </c>
       <c r="P3" s="1">
-        <v>1.02</v>
+        <v>1.423</v>
       </c>
       <c r="Q3" s="1">
-        <v>0.47099999999999997</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="R3" s="1">
-        <v>0.76800000000000002</v>
+        <v>0.93</v>
       </c>
       <c r="S3" s="1">
-        <v>0.47399999999999998</v>
+        <v>0.501</v>
       </c>
       <c r="T3" s="1">
-        <v>1.526</v>
+        <v>1.3979999999999999</v>
       </c>
       <c r="U3" s="1">
-        <v>0.64600000000000002</v>
+        <v>0.626</v>
       </c>
       <c r="V3" s="1">
-        <v>0.44</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="W3" s="1">
-        <v>0.55600000000000005</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="X3" s="1">
-        <v>0.61499999999999999</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="Y3" s="1">
-        <v>0.40300000000000002</v>
+        <v>0.42</v>
       </c>
       <c r="Z3" s="1">
-        <v>0.45100000000000001</v>
+        <v>0.496</v>
       </c>
       <c r="AA3" s="1">
-        <v>0.46500000000000002</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1">
-        <v>0.44400000000000001</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="AD3" s="1">
-        <v>0.53500000000000003</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE3" s="1">
-        <v>0.48199999999999998</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1">
-        <v>0.41</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="AH3" s="1">
-        <v>0.48</v>
+        <v>0.433</v>
       </c>
       <c r="AI3" s="1">
-        <v>0.66100000000000003</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0.499</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="AK3" s="1">
-        <v>0.44400000000000001</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="AL3" s="1">
-        <v>1.2689999999999999</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="AM3" s="1">
-        <v>0.43099999999999999</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="AN3" s="1">
-        <v>0.45200000000000001</v>
+        <v>0.51900000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>0.99</v>
+        <v>1.069</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>0.72299999999999998</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
-        <v>0.47099999999999997</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1">
-        <v>0.54900000000000004</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="N4" s="1">
-        <v>0.64</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="O4" s="1">
-        <v>4.2359999999999998</v>
+        <v>2.742</v>
       </c>
       <c r="P4" s="1">
-        <v>1.423</v>
+        <v>1.744</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.44600000000000001</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="R4" s="1">
-        <v>0.93</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="S4" s="1">
-        <v>0.501</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="T4" s="1">
-        <v>1.3979999999999999</v>
+        <v>1.5780000000000001</v>
       </c>
       <c r="U4" s="1">
-        <v>0.626</v>
+        <v>0.499</v>
       </c>
       <c r="V4" s="1">
-        <v>0.49099999999999999</v>
+        <v>0.497</v>
       </c>
       <c r="W4" s="1">
-        <v>0.43099999999999999</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="X4" s="1">
-        <v>0.52300000000000002</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="Y4" s="1">
-        <v>0.42</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="Z4" s="1">
-        <v>0.496</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="AA4" s="1">
-        <v>0.42399999999999999</v>
+        <v>0.433</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1">
-        <v>0.40500000000000003</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="AD4" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="AE4" s="1">
-        <v>0.40300000000000002</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1">
-        <v>0.40100000000000002</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="AH4" s="1">
-        <v>0.433</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="AI4" s="1">
-        <v>0.63300000000000001</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0.54200000000000004</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="AK4" s="1">
-        <v>0.40500000000000003</v>
+        <v>0.376</v>
       </c>
       <c r="AL4" s="1">
-        <v>0.97299999999999998</v>
+        <v>1.01</v>
       </c>
       <c r="AM4" s="1">
-        <v>0.42499999999999999</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="AN4" s="1">
-        <v>0.51900000000000002</v>
+        <v>0.40899999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1.069</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <v>0.79500000000000004</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1">
-        <v>0.51400000000000001</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1">
-        <v>0.70799999999999996</v>
+        <v>0.65</v>
       </c>
       <c r="N5" s="1">
-        <v>0.58599999999999997</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="O5" s="1">
-        <v>2.742</v>
+        <v>3.01</v>
       </c>
       <c r="P5" s="1">
-        <v>1.744</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.44700000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="R5" s="1">
-        <v>0.91800000000000004</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="S5" s="1">
-        <v>0.48699999999999999</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="T5" s="1">
-        <v>1.5780000000000001</v>
+        <v>1.617</v>
       </c>
       <c r="U5" s="1">
-        <v>0.499</v>
+        <v>0.622</v>
       </c>
       <c r="V5" s="1">
-        <v>0.497</v>
+        <v>0.498</v>
       </c>
       <c r="W5" s="1">
-        <v>0.47099999999999997</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="X5" s="1">
-        <v>0.48399999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="Y5" s="1">
-        <v>0.45500000000000002</v>
+        <v>0.434</v>
       </c>
       <c r="Z5" s="1">
-        <v>0.45500000000000002</v>
+        <v>0.502</v>
       </c>
       <c r="AA5" s="1">
-        <v>0.433</v>
+        <v>0.503</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1">
-        <v>0.41099999999999998</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="AD5" s="1">
-        <v>0.46100000000000002</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="AE5" s="1">
-        <v>0.46899999999999997</v>
+        <v>0.501</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1">
-        <v>0.47799999999999998</v>
+        <v>0.39</v>
       </c>
       <c r="AH5" s="1">
-        <v>0.38600000000000001</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="AI5" s="1">
-        <v>0.72099999999999997</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0.52200000000000002</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="AK5" s="1">
-        <v>0.376</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="AL5" s="1">
-        <v>1.01</v>
+        <v>0.78600000000000003</v>
       </c>
       <c r="AM5" s="1">
-        <v>0.39900000000000002</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="AN5" s="1">
-        <v>0.40899999999999997</v>
+        <v>0.41099999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1.1579999999999999</v>
+        <v>1.0940000000000001</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>0.60099999999999998</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1">
-        <v>0.54200000000000004</v>
+        <v>0.43</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1">
-        <v>0.65</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="N6" s="1">
-        <v>0.64500000000000002</v>
+        <v>0.504</v>
       </c>
       <c r="O6" s="1">
-        <v>3.01</v>
+        <v>4.2690000000000001</v>
       </c>
       <c r="P6" s="1">
-        <v>1.7250000000000001</v>
+        <v>1.3740000000000001</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.45</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="R6" s="1">
-        <v>0.67100000000000004</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="S6" s="1">
-        <v>0.54800000000000004</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="T6" s="1">
-        <v>1.617</v>
+        <v>1.581</v>
       </c>
       <c r="U6" s="1">
-        <v>0.622</v>
+        <v>0.623</v>
       </c>
       <c r="V6" s="1">
-        <v>0.498</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="W6" s="1">
-        <v>0.40300000000000002</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="X6" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="Y6" s="1">
-        <v>0.434</v>
+        <v>0.441</v>
       </c>
       <c r="Z6" s="1">
         <v>0.502</v>
       </c>
       <c r="AA6" s="1">
-        <v>0.503</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1">
-        <v>0.42299999999999999</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="AD6" s="1">
-        <v>0.54600000000000004</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="AE6" s="1">
-        <v>0.501</v>
+        <v>0.443</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1">
-        <v>0.39</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="AH6" s="1">
-        <v>0.43099999999999999</v>
+        <v>0.437</v>
       </c>
       <c r="AI6" s="1">
-        <v>0.59699999999999998</v>
+        <v>0.63</v>
       </c>
       <c r="AJ6" s="1">
-        <v>0.50800000000000001</v>
+        <v>0.437</v>
       </c>
       <c r="AK6" s="1">
-        <v>0.41699999999999998</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="AL6" s="1">
-        <v>0.78600000000000003</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="AM6" s="1">
-        <v>0.45400000000000001</v>
+        <v>0.434</v>
       </c>
       <c r="AN6" s="1">
-        <v>0.41099999999999998</v>
+        <v>0.44900000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1.0940000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>0.58799999999999997</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1">
-        <v>0.43</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1">
-        <v>0.58899999999999997</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="N7" s="1">
-        <v>0.504</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="O7" s="1">
-        <v>4.2690000000000001</v>
+        <v>3.319</v>
       </c>
       <c r="P7" s="1">
-        <v>1.3740000000000001</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="Q7" s="1">
-        <v>0.41499999999999998</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="R7" s="1">
-        <v>0.65800000000000003</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="S7" s="1">
-        <v>0.48699999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="T7" s="1">
-        <v>1.581</v>
+        <v>1.5589999999999999</v>
       </c>
       <c r="U7" s="1">
-        <v>0.623</v>
+        <v>0.755</v>
       </c>
       <c r="V7" s="1">
-        <v>0.53300000000000003</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="W7" s="1">
-        <v>0.44400000000000001</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="X7" s="1">
-        <v>0.55100000000000005</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="Y7" s="1">
-        <v>0.441</v>
+        <v>0.435</v>
       </c>
       <c r="Z7" s="1">
-        <v>0.502</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="AA7" s="1">
-        <v>0.46700000000000003</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1">
-        <v>0.49099999999999999</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="AD7" s="1">
-        <v>0.54700000000000004</v>
+        <v>0.52</v>
       </c>
       <c r="AE7" s="1">
-        <v>0.443</v>
+        <v>0.48</v>
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1">
-        <v>0.47899999999999998</v>
+        <v>0.436</v>
       </c>
       <c r="AH7" s="1">
-        <v>0.437</v>
+        <v>0.441</v>
       </c>
       <c r="AI7" s="1">
-        <v>0.63</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0.437</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="AK7" s="1">
-        <v>0.39500000000000002</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="AL7" s="1">
-        <v>0.88300000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="AM7" s="1">
-        <v>0.434</v>
+        <v>0.432</v>
       </c>
       <c r="AN7" s="1">
-        <v>0.44900000000000001</v>
+        <v>0.45400000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.123</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <v>0.60899999999999999</v>
+        <v>0.625</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1">
-        <v>0.58299999999999996</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1">
-        <v>0.68100000000000005</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="N8" s="1">
-        <v>0.47099999999999997</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="O8" s="1">
-        <v>3.319</v>
+        <v>3.879</v>
       </c>
       <c r="P8" s="1">
-        <v>0.93600000000000005</v>
+        <v>1.845</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.45400000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="R8" s="1">
-        <v>0.60399999999999998</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="S8" s="1">
-        <v>0.5</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="T8" s="1">
-        <v>1.5589999999999999</v>
+        <v>1.4870000000000001</v>
       </c>
       <c r="U8" s="1">
-        <v>0.755</v>
+        <v>0.64</v>
       </c>
       <c r="V8" s="1">
-        <v>0.47799999999999998</v>
+        <v>1.1739999999999999</v>
       </c>
       <c r="W8" s="1">
-        <v>0.39300000000000002</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="X8" s="1">
-        <v>0.56599999999999995</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="Y8" s="1">
-        <v>0.435</v>
+        <v>0.44</v>
       </c>
       <c r="Z8" s="1">
-        <v>0.45600000000000002</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="AA8" s="1">
-        <v>0.53900000000000003</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1">
-        <v>0.35399999999999998</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="AD8" s="1">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="AE8" s="1">
-        <v>0.48</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1">
-        <v>0.436</v>
+        <v>0.45</v>
       </c>
       <c r="AH8" s="1">
-        <v>0.441</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="AI8" s="1">
-        <v>0.63900000000000001</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="AJ8" s="1">
-        <v>0.51300000000000001</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="AK8" s="1">
-        <v>0.60599999999999998</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="AL8" s="1">
-        <v>0.92</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="AM8" s="1">
-        <v>0.432</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="AN8" s="1">
-        <v>0.45400000000000001</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>1.123</v>
+        <v>1.103</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <v>0.625</v>
+        <v>0.621</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1">
-        <v>0.51700000000000002</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1">
-        <v>0.64100000000000001</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="N9" s="1">
-        <v>0.83599999999999997</v>
+        <v>0.83</v>
       </c>
       <c r="O9" s="1">
-        <v>3.879</v>
+        <v>2.702</v>
       </c>
       <c r="P9" s="1">
-        <v>1.845</v>
+        <v>1.1160000000000001</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.44</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="R9" s="1">
-        <v>0.82699999999999996</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="S9" s="1">
-        <v>0.41699999999999998</v>
+        <v>0.46</v>
       </c>
       <c r="T9" s="1">
-        <v>1.4870000000000001</v>
+        <v>1.391</v>
       </c>
       <c r="U9" s="1">
-        <v>0.64</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="V9" s="1">
-        <v>1.1739999999999999</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="W9" s="1">
-        <v>0.55200000000000005</v>
+        <v>0.502</v>
       </c>
       <c r="X9" s="1">
-        <v>0.59899999999999998</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="Y9" s="1">
-        <v>0.44</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="Z9" s="1">
-        <v>0.55200000000000005</v>
+        <v>0.442</v>
       </c>
       <c r="AA9" s="1">
-        <v>0.48499999999999999</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1">
-        <v>0.52300000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="AD9" s="1">
-        <v>0.54</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="AE9" s="1">
-        <v>0.40200000000000002</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="AK9" s="1">
         <v>0.45</v>
       </c>
-      <c r="AH9" s="1">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="AI9" s="1">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="AJ9" s="1">
-        <v>0.57199999999999995</v>
-      </c>
-      <c r="AK9" s="1">
-        <v>0.52600000000000002</v>
-      </c>
       <c r="AL9" s="1">
-        <v>0.95899999999999996</v>
+        <v>1.042</v>
       </c>
       <c r="AM9" s="1">
-        <v>0.53400000000000003</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="AN9" s="1">
-        <v>0.4</v>
+        <v>0.48399999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>1.103</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
-        <v>0.621</v>
+        <v>0.59</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1">
-        <v>0.44700000000000001</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1">
-        <v>0.55500000000000005</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="N10" s="1">
-        <v>0.83</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="O10" s="1">
-        <v>2.702</v>
+        <v>2.7160000000000002</v>
       </c>
       <c r="P10" s="1">
-        <v>1.1160000000000001</v>
+        <v>1.5509999999999999</v>
       </c>
       <c r="Q10" s="1">
-        <v>0.41599999999999998</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="R10" s="1">
-        <v>0.61099999999999999</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="S10" s="1">
-        <v>0.46</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="T10" s="1">
-        <v>1.391</v>
+        <v>1.3260000000000001</v>
       </c>
       <c r="U10" s="1">
-        <v>0.70199999999999996</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="V10" s="1">
-        <v>0.46899999999999997</v>
+        <v>0.43</v>
       </c>
       <c r="W10" s="1">
-        <v>0.502</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="X10" s="1">
-        <v>0.56699999999999995</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="Y10" s="1">
-        <v>0.39600000000000002</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="Z10" s="1">
-        <v>0.442</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="AA10" s="1">
-        <v>0.51900000000000002</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1">
-        <v>0.375</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD10" s="1">
-        <v>0.59199999999999997</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="AE10" s="1">
-        <v>0.45500000000000002</v>
+        <v>0.43</v>
       </c>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1">
-        <v>0.53400000000000003</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="AH10" s="1">
-        <v>0.41799999999999998</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="AI10" s="1">
-        <v>0.76200000000000001</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="AJ10" s="1">
-        <v>0.54</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="AK10" s="1">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="AL10" s="1">
-        <v>1.042</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="AM10" s="1">
-        <v>0.42899999999999999</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="AN10" s="1">
-        <v>0.48399999999999999</v>
+        <v>0.41599999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>0.99399999999999999</v>
+        <v>1.133</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
-        <v>0.59</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1">
-        <v>0.49199999999999999</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1">
-        <v>0.59299999999999997</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="N11" s="1">
-        <v>0.81200000000000006</v>
+        <v>1.081</v>
       </c>
       <c r="O11" s="1">
-        <v>2.7160000000000002</v>
+        <v>2.7829999999999999</v>
       </c>
       <c r="P11" s="1">
-        <v>1.5509999999999999</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0.42899999999999999</v>
-      </c>
+        <v>1.335</v>
+      </c>
+      <c r="Q11" s="1"/>
       <c r="R11" s="1">
-        <v>0.83499999999999996</v>
+        <v>0.85099999999999998</v>
       </c>
       <c r="S11" s="1">
-        <v>0.55300000000000005</v>
+        <v>0.52</v>
       </c>
       <c r="T11" s="1">
-        <v>1.3260000000000001</v>
+        <v>1.458</v>
       </c>
       <c r="U11" s="1">
-        <v>0.61899999999999999</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="V11" s="1">
-        <v>0.43</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="W11" s="1">
-        <v>0.45100000000000001</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="X11" s="1">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="AA11" s="1">
         <v>0.53900000000000003</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>0.47299999999999998</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>0.52400000000000002</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="AD11" s="1">
-        <v>0.63600000000000001</v>
+        <v>0.63100000000000001</v>
       </c>
       <c r="AE11" s="1">
-        <v>0.43</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1">
-        <v>0.48899999999999999</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="AH11" s="1">
-        <v>0.39700000000000002</v>
+        <v>0.441</v>
       </c>
       <c r="AI11" s="1">
-        <v>0.58499999999999996</v>
+        <v>0.72</v>
       </c>
       <c r="AJ11" s="1">
-        <v>0.53700000000000003</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="AK11" s="1">
-        <v>0.43</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="AL11" s="1">
-        <v>0.92700000000000005</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="AM11" s="1">
-        <v>0.50900000000000001</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="AN11" s="1">
-        <v>0.41599999999999998</v>
+        <v>0.53300000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>1.133</v>
+        <v>1.1879999999999999</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
-        <v>0.71199999999999997</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1">
-        <v>0.48399999999999999</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1">
-        <v>0.60699999999999998</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="N12" s="1">
-        <v>1.081</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="O12" s="1">
-        <v>2.7829999999999999</v>
+        <v>3.8820000000000001</v>
       </c>
       <c r="P12" s="1">
-        <v>1.335</v>
+        <v>1.4510000000000001</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1">
-        <v>0.85099999999999998</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="S12" s="1">
-        <v>0.52</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="T12" s="1">
-        <v>1.458</v>
+        <v>1.3919999999999999</v>
       </c>
       <c r="U12" s="1">
-        <v>0.51400000000000001</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="V12" s="1">
-        <v>0.48799999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="W12" s="1">
-        <v>0.41499999999999998</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="X12" s="1">
-        <v>0.52200000000000002</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="Y12" s="1">
-        <v>0.42399999999999999</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="Z12" s="1">
-        <v>0.47399999999999998</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="AA12" s="1">
-        <v>0.53900000000000003</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="AD12" s="1">
-        <v>0.63100000000000001</v>
-      </c>
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="AD12" s="1"/>
       <c r="AE12" s="1">
-        <v>0.36099999999999999</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1">
-        <v>0.55200000000000005</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="AH12" s="1">
-        <v>0.441</v>
+        <v>0.376</v>
       </c>
       <c r="AI12" s="1">
-        <v>0.72</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="AJ12" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="AK12" s="1">
-        <v>0.50800000000000001</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="AL12" s="1">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="AM12" s="1">
-        <v>0.40200000000000002</v>
-      </c>
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="AM12" s="1"/>
       <c r="AN12" s="1">
-        <v>0.53300000000000003</v>
+        <v>0.503</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>1.1879999999999999</v>
+        <v>1.155</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
-        <v>0.66900000000000004</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1793,90 +1774,80 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1">
-        <v>0.57199999999999995</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="N13" s="1">
-        <v>0.77400000000000002</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="O13" s="1">
-        <v>3.8820000000000001</v>
+        <v>2.907</v>
       </c>
       <c r="P13" s="1">
-        <v>1.4510000000000001</v>
+        <v>1.4970000000000001</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1">
-        <v>0.80800000000000005</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="S13" s="1">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="T13" s="1">
-        <v>1.3919999999999999</v>
-      </c>
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T13" s="1"/>
       <c r="U13" s="1">
-        <v>0.65200000000000002</v>
+        <v>0.6</v>
       </c>
       <c r="V13" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="W13" s="1">
-        <v>0.40899999999999997</v>
-      </c>
+        <v>0.46</v>
+      </c>
+      <c r="W13" s="1"/>
       <c r="X13" s="1">
-        <v>0.52800000000000002</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="Y13" s="1">
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>0.48899999999999999</v>
-      </c>
+        <v>0.439</v>
+      </c>
+      <c r="Z13" s="1"/>
       <c r="AA13" s="1">
-        <v>0.40200000000000002</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1">
-        <v>0.51400000000000001</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="AD13" s="1"/>
-      <c r="AE13" s="1">
-        <v>0.40400000000000003</v>
-      </c>
+      <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
       <c r="AG13" s="1">
-        <v>0.47699999999999998</v>
+        <v>0.441</v>
       </c>
       <c r="AH13" s="1">
-        <v>0.376</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="AI13" s="1">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="AJ13" s="1">
         <v>0.67200000000000004</v>
       </c>
+      <c r="AJ13" s="1"/>
       <c r="AK13" s="1">
-        <v>0.42899999999999999</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="AL13" s="1">
-        <v>0.82899999999999996</v>
+        <v>1.016</v>
       </c>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1">
-        <v>0.503</v>
+        <v>0.42399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>1.155</v>
+        <v>1.127</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
-        <v>0.68799999999999994</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1885,80 +1856,72 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1">
-        <v>0.57799999999999996</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="N14" s="1">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="O14" s="1">
-        <v>2.907</v>
-      </c>
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="O14" s="1"/>
       <c r="P14" s="1">
-        <v>1.4970000000000001</v>
+        <v>1.581</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1">
-        <v>1.0129999999999999</v>
+        <v>0.84</v>
       </c>
       <c r="S14" s="1">
-        <v>0.42399999999999999</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1">
-        <v>0.6</v>
+        <v>0.73</v>
       </c>
       <c r="V14" s="1">
-        <v>0.46</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="W14" s="1"/>
-      <c r="X14" s="1">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="Y14" s="1">
-        <v>0.439</v>
-      </c>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1">
-        <v>0.55500000000000005</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1">
-        <v>0.46899999999999997</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1">
-        <v>0.441</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="AH14" s="1">
-        <v>0.40100000000000002</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="AI14" s="1">
-        <v>0.67200000000000004</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1">
-        <v>0.44600000000000001</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="AL14" s="1">
-        <v>1.016</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="AM14" s="1"/>
-      <c r="AN14" s="1">
-        <v>0.42399999999999999</v>
-      </c>
+      <c r="AN14" s="1"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>1.127</v>
+        <v>1.1419999999999999</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
-        <v>0.64700000000000002</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1967,73 +1930,67 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1">
-        <v>0.57499999999999996</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="N15" s="1">
-        <v>0.71399999999999997</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1">
-        <v>1.581</v>
+        <v>1.2709999999999999</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1">
-        <v>0.84</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="S15" s="1">
-        <v>0.46800000000000003</v>
+        <v>0.49</v>
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1">
-        <v>0.73</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="V15" s="1">
-        <v>0.51300000000000001</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1">
-        <v>0.53600000000000003</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1">
-        <v>0.39600000000000002</v>
+        <v>0.374</v>
       </c>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="AH15" s="1">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="AI15" s="1">
-        <v>0.73799999999999999</v>
-      </c>
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1">
-        <v>0.46300000000000002</v>
+        <v>0.43</v>
       </c>
       <c r="AL15" s="1">
-        <v>0.93799999999999994</v>
+        <v>1.1379999999999999</v>
       </c>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>1.1419999999999999</v>
+        <v>1.2290000000000001</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <v>0.55600000000000005</v>
-      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2041,61 +1998,55 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1">
-        <v>0.61899999999999999</v>
+        <v>0.70699999999999996</v>
       </c>
       <c r="N16" s="1">
-        <v>0.65600000000000003</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="O16" s="1"/>
-      <c r="P16" s="1">
-        <v>1.2709999999999999</v>
-      </c>
+      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1">
-        <v>0.99399999999999999</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="S16" s="1">
-        <v>0.49</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1">
-        <v>0.84799999999999998</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="V16" s="1">
-        <v>0.42299999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1">
-        <v>0.47699999999999998</v>
+        <v>0.495</v>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1">
-        <v>0.374</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
-      <c r="AG16" s="1">
-        <v>0.47399999999999998</v>
-      </c>
+      <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
-      <c r="AK16" s="1">
-        <v>0.43</v>
-      </c>
+      <c r="AK16" s="1"/>
       <c r="AL16" s="1">
-        <v>1.1379999999999999</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>1.2290000000000001</v>
+        <v>1.1919999999999999</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2109,38 +2060,32 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1">
-        <v>0.70699999999999996</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="N17" s="1">
-        <v>0.82599999999999996</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1">
-        <v>0.97699999999999998</v>
+        <v>0.84299999999999997</v>
       </c>
       <c r="S17" s="1">
-        <v>0.39800000000000002</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="T17" s="1"/>
-      <c r="U17" s="1">
-        <v>0.70099999999999996</v>
-      </c>
+      <c r="U17" s="1"/>
       <c r="V17" s="1">
-        <v>0.46500000000000002</v>
+        <v>0.48</v>
       </c>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="1">
-        <v>0.495</v>
-      </c>
+      <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="1">
-        <v>0.47599999999999998</v>
-      </c>
+      <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
@@ -2150,14 +2095,14 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1">
-        <v>1.0649999999999999</v>
+        <v>1.32</v>
       </c>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>1.1919999999999999</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2171,24 +2116,24 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1">
-        <v>0.58899999999999997</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="N18" s="1">
-        <v>0.72599999999999998</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1">
-        <v>0.84299999999999997</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="S18" s="1">
-        <v>0.49299999999999999</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1">
-        <v>0.48</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -2205,16 +2150,12 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
-      <c r="AL18" s="1">
-        <v>1.32</v>
-      </c>
+      <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1.0149999999999999</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2227,25 +2168,21 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1">
-        <v>0.59799999999999998</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="N19" s="1">
-        <v>0.59099999999999997</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1">
-        <v>0.78300000000000003</v>
-      </c>
-      <c r="S19" s="1">
-        <v>0.57099999999999995</v>
-      </c>
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-      <c r="V19" s="1">
-        <v>0.44800000000000001</v>
-      </c>
+      <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -2279,16 +2216,16 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1">
-        <v>0.56699999999999995</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="N20" s="1">
-        <v>0.71899999999999997</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1">
-        <v>0.80600000000000005</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -2314,29 +2251,37 @@
       <c r="AN20" s="1"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="1">
+        <v>1.486</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.8009999999999999</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>0.64400000000000002</v>
+      </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1">
+        <v>0.43</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1">
-        <v>0.59699999999999998</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="N21" s="1">
-        <v>0.52200000000000002</v>
+        <v>1.014</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1">
-        <v>0.73299999999999998</v>
+        <v>0.81399999999999995</v>
       </c>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -2363,19 +2308,19 @@
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>1.486</v>
+        <v>1.355</v>
       </c>
       <c r="B22" s="1">
-        <v>1.8009999999999999</v>
+        <v>1.706</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1">
-        <v>0.64400000000000002</v>
+        <v>0.73</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <v>0.43</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2383,17 +2328,15 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1">
-        <v>0.60799999999999998</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="N22" s="1">
-        <v>1.014</v>
+        <v>0.63100000000000001</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1">
-        <v>0.81399999999999995</v>
-      </c>
+      <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -2419,30 +2362,28 @@
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>1.355</v>
+        <v>1.518</v>
       </c>
       <c r="B23" s="1">
-        <v>1.706</v>
+        <v>1.77</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1">
-        <v>0.73</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1">
-        <v>0.41399999999999998</v>
+        <v>0.501</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1">
-        <v>0.54100000000000004</v>
-      </c>
+      <c r="M23" s="1"/>
       <c r="N23" s="1">
-        <v>0.63100000000000001</v>
+        <v>0.749</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2473,29 +2414,29 @@
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>1.518</v>
+        <v>1.369</v>
       </c>
       <c r="B24" s="1">
-        <v>1.77</v>
+        <v>1.954</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
-        <v>0.66900000000000004</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1">
-        <v>0.501</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1">
-        <v>0.749</v>
-      </c>
+      <c r="M24" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2525,19 +2466,19 @@
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>1.369</v>
+        <v>1.3819999999999999</v>
       </c>
       <c r="B25" s="1">
-        <v>1.954</v>
+        <v>1.708</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1">
-        <v>0.51100000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
-        <v>0.41799999999999998</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2545,7 +2486,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1">
-        <v>0.59</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -2577,19 +2518,19 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>1.3819999999999999</v>
+        <v>1.421</v>
       </c>
       <c r="B26" s="1">
-        <v>1.708</v>
+        <v>1.387</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
-        <v>0.67</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
-        <v>0.41899999999999998</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2597,7 +2538,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1">
-        <v>0.61499999999999999</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -2629,19 +2570,19 @@
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>1.421</v>
+        <v>1.6379999999999999</v>
       </c>
       <c r="B27" s="1">
-        <v>1.387</v>
+        <v>1.7470000000000001</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
-        <v>0.65700000000000003</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
-        <v>0.46300000000000002</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2649,7 +2590,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -2681,19 +2622,19 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>1.6379999999999999</v>
+        <v>1.556</v>
       </c>
       <c r="B28" s="1">
-        <v>1.7470000000000001</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
-        <v>0.67900000000000005</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1">
-        <v>0.46200000000000002</v>
+        <v>0.372</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2701,7 +2642,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1">
-        <v>0.52200000000000002</v>
+        <v>0.64</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -2733,27 +2674,23 @@
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>1.556</v>
+        <v>1.464</v>
       </c>
       <c r="B29" s="1">
-        <v>0.94899999999999995</v>
+        <v>1.8660000000000001</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1">
-        <v>0.67200000000000004</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1">
-        <v>0.372</v>
-      </c>
+      <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1">
-        <v>0.64</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -2785,11 +2722,9 @@
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>1.464</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.8660000000000001</v>
-      </c>
+        <v>1.653</v>
+      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -2801,7 +2736,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1">
-        <v>0.69199999999999995</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2833,7 +2768,7 @@
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>1.653</v>
+        <v>1.631</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2847,7 +2782,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1">
-        <v>0.78400000000000003</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2879,7 +2814,7 @@
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>1.631</v>
+        <v>1.7030000000000001</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2893,7 +2828,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -2925,7 +2860,7 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>1.7030000000000001</v>
+        <v>1.9610000000000001</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2939,7 +2874,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1">
-        <v>0.59699999999999998</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -2970,9 +2905,7 @@
       <c r="AN33" s="1"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>1.9610000000000001</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2985,7 +2918,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1">
-        <v>0.59299999999999997</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -3029,7 +2962,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1">
-        <v>0.61099999999999999</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -3073,7 +3006,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1">
-        <v>0.58699999999999997</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -3104,20 +3037,38 @@
       <c r="AN36" s="1"/>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="A37" s="1">
+        <v>1.5189999999999999</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.7969999999999999</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.46800000000000003</v>
+      </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="I37" s="1">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.46800000000000003</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1">
-        <v>0.61099999999999999</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -3149,37 +3100,37 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>1.5189999999999999</v>
+        <v>1.677</v>
       </c>
       <c r="B38" s="1">
-        <v>1.7969999999999999</v>
+        <v>1.397</v>
       </c>
       <c r="C38" s="1">
-        <v>0.95599999999999996</v>
+        <v>1.079</v>
       </c>
       <c r="D38" s="1">
-        <v>0.83199999999999996</v>
+        <v>0.92</v>
       </c>
       <c r="E38" s="1">
-        <v>0.66900000000000004</v>
+        <v>0.64</v>
       </c>
       <c r="F38" s="1">
-        <v>0.66400000000000003</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="G38" s="1">
-        <v>0.46800000000000003</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1">
-        <v>0.63900000000000001</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="J38" s="1">
-        <v>0.46800000000000003</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1">
-        <v>0.60299999999999998</v>
+        <v>0.53</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -3211,37 +3162,37 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>1.677</v>
+        <v>1.2609999999999999</v>
       </c>
       <c r="B39" s="1">
-        <v>1.397</v>
+        <v>1.554</v>
       </c>
       <c r="C39" s="1">
-        <v>1.079</v>
+        <v>1.052</v>
       </c>
       <c r="D39" s="1">
-        <v>0.92</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="E39" s="1">
-        <v>0.64</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="F39" s="1">
-        <v>0.68200000000000005</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="G39" s="1">
-        <v>0.51300000000000001</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1">
-        <v>0.57199999999999995</v>
+        <v>0.5</v>
       </c>
       <c r="J39" s="1">
-        <v>0.45200000000000001</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1">
-        <v>0.53</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -3273,38 +3224,36 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>1.2609999999999999</v>
+        <v>1.605</v>
       </c>
       <c r="B40" s="1">
-        <v>1.554</v>
+        <v>2.0419999999999998</v>
       </c>
       <c r="C40" s="1">
-        <v>1.052</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="D40" s="1">
-        <v>0.84599999999999997</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="E40" s="1">
-        <v>0.68500000000000005</v>
+        <v>0.64</v>
       </c>
       <c r="F40" s="1">
-        <v>0.67300000000000004</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="G40" s="1">
-        <v>0.54600000000000004</v>
+        <v>0.44</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1">
-        <v>0.5</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="J40" s="1">
-        <v>0.46500000000000002</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="1">
-        <v>0.65700000000000003</v>
-      </c>
+      <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -3335,32 +3284,32 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>1.605</v>
+        <v>1.369</v>
       </c>
       <c r="B41" s="1">
-        <v>2.0419999999999998</v>
+        <v>2.149</v>
       </c>
       <c r="C41" s="1">
-        <v>0.97299999999999998</v>
+        <v>1.1379999999999999</v>
       </c>
       <c r="D41" s="1">
-        <v>0.96499999999999997</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="E41" s="1">
-        <v>0.64</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="F41" s="1">
-        <v>0.70599999999999996</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G41" s="1">
-        <v>0.44</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1">
-        <v>0.51800000000000002</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="J41" s="1">
-        <v>0.45700000000000002</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -3395,32 +3344,32 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>1.369</v>
+        <v>1.389</v>
       </c>
       <c r="B42" s="1">
-        <v>2.149</v>
+        <v>1.841</v>
       </c>
       <c r="C42" s="1">
-        <v>1.1379999999999999</v>
+        <v>1.097</v>
       </c>
       <c r="D42" s="1">
-        <v>0.94899999999999995</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="E42" s="1">
-        <v>0.79400000000000004</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="F42" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="G42" s="1">
-        <v>0.42599999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1">
-        <v>0.66100000000000003</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="J42" s="1">
-        <v>0.64500000000000002</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -3455,32 +3404,30 @@
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>1.389</v>
+        <v>1.6060000000000001</v>
       </c>
       <c r="B43" s="1">
-        <v>1.841</v>
+        <v>1.9450000000000001</v>
       </c>
       <c r="C43" s="1">
-        <v>1.097</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D43" s="1">
-        <v>0.93300000000000005</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="E43" s="1">
-        <v>0.57099999999999995</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="F43" s="1">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="G43" s="1">
-        <v>0.49</v>
-      </c>
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1">
-        <v>0.48399999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="J43" s="1">
-        <v>0.44400000000000001</v>
+        <v>0.502</v>
       </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -3515,30 +3462,30 @@
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>1.6060000000000001</v>
+        <v>1.28</v>
       </c>
       <c r="B44" s="1">
-        <v>1.9450000000000001</v>
+        <v>2.0640000000000001</v>
       </c>
       <c r="C44" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="D44" s="1">
-        <v>0.94099999999999995</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="E44" s="1">
-        <v>0.53200000000000003</v>
+        <v>0.65</v>
       </c>
       <c r="F44" s="1">
-        <v>0.56799999999999995</v>
+        <v>0.69</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1">
-        <v>0.59</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="J44" s="1">
-        <v>0.502</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -3573,22 +3520,22 @@
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>1.28</v>
+        <v>1.4370000000000001</v>
       </c>
       <c r="B45" s="1">
-        <v>2.0640000000000001</v>
+        <v>1.851</v>
       </c>
       <c r="C45" s="1">
-        <v>1.2310000000000001</v>
+        <v>1.0640000000000001</v>
       </c>
       <c r="D45" s="1">
-        <v>0.83699999999999997</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="E45" s="1">
-        <v>0.65</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="F45" s="1">
-        <v>0.69</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -3596,7 +3543,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="J45" s="1">
-        <v>0.57799999999999996</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -3631,30 +3578,30 @@
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>1.4370000000000001</v>
+        <v>1.623</v>
       </c>
       <c r="B46" s="1">
-        <v>1.851</v>
+        <v>1.927</v>
       </c>
       <c r="C46" s="1">
-        <v>1.0640000000000001</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="D46" s="1">
-        <v>0.98099999999999998</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="E46" s="1">
-        <v>0.68600000000000005</v>
+        <v>0.59899999999999998</v>
       </c>
       <c r="F46" s="1">
-        <v>0.71099999999999997</v>
+        <v>0.621</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1">
-        <v>0.60799999999999998</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="J46" s="1">
-        <v>0.46700000000000003</v>
+        <v>0.49</v>
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -3689,30 +3636,28 @@
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>1.623</v>
+        <v>1.1259999999999999</v>
       </c>
       <c r="B47" s="1">
-        <v>1.927</v>
-      </c>
-      <c r="C47" s="1">
-        <v>0.93799999999999994</v>
-      </c>
+        <v>1.74</v>
+      </c>
+      <c r="C47" s="1"/>
       <c r="D47" s="1">
-        <v>0.77300000000000002</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="E47" s="1">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="F47" s="1">
         <v>0.59899999999999998</v>
-      </c>
-      <c r="F47" s="1">
-        <v>0.621</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1">
-        <v>0.48599999999999999</v>
+        <v>0.499</v>
       </c>
       <c r="J47" s="1">
-        <v>0.49</v>
+        <v>0.497</v>
       </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -3747,28 +3692,28 @@
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>1.1259999999999999</v>
+        <v>1.4410000000000001</v>
       </c>
       <c r="B48" s="1">
-        <v>1.74</v>
+        <v>1.7190000000000001</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
-        <v>0.88500000000000001</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="E48" s="1">
-        <v>0.67900000000000005</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="F48" s="1">
-        <v>0.59899999999999998</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1">
-        <v>0.499</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="J48" s="1">
-        <v>0.497</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -3803,28 +3748,26 @@
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>1.4410000000000001</v>
-      </c>
-      <c r="B49" s="1">
-        <v>1.7190000000000001</v>
-      </c>
+        <v>1.125</v>
+      </c>
+      <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1">
-        <v>0.85399999999999998</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="E49" s="1">
-        <v>0.66900000000000004</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="F49" s="1">
-        <v>0.66800000000000004</v>
+        <v>0.621</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1">
-        <v>0.58299999999999996</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="J49" s="1">
-        <v>0.47799999999999998</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -3859,26 +3802,24 @@
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>1.125</v>
+        <v>1.474</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="E50" s="1">
-        <v>0.72199999999999998</v>
-      </c>
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="1">
-        <v>0.621</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1">
-        <v>0.70599999999999996</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="J50" s="1">
-        <v>0.52300000000000002</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -3912,26 +3853,20 @@
       <c r="AN50" s="1"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>1.474</v>
-      </c>
+      <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1">
-        <v>0.82299999999999995</v>
+        <v>1.337</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="F51" s="1">
-        <v>0.58699999999999997</v>
-      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="J51" s="1">
-        <v>0.52800000000000002</v>
-      </c>
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -3968,14 +3903,14 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1">
-        <v>1.337</v>
+        <v>1.006</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1">
-        <v>0.61599999999999999</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -4013,15 +3948,13 @@
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="1">
-        <v>1.006</v>
-      </c>
+      <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1">
-        <v>0.53400000000000003</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -4065,7 +3998,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1">
-        <v>0.48799999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -4109,7 +4042,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1">
-        <v>0.49399999999999999</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -4153,7 +4086,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1">
-        <v>0.51500000000000001</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
@@ -4197,7 +4130,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -4240,9 +4173,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="1">
-        <v>0.60399999999999998</v>
-      </c>
+      <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -4326,7 +4257,9 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
+      <c r="I60" s="1">
+        <v>0.64300000000000002</v>
+      </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -4369,7 +4302,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1">
-        <v>0.64300000000000002</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -4413,7 +4346,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1">
-        <v>0.58699999999999997</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -4457,7 +4390,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1">
-        <v>0.58399999999999996</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -4501,7 +4434,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1">
-        <v>0.64300000000000002</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -4545,7 +4478,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1">
-        <v>0.59799999999999998</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -4589,7 +4522,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1">
-        <v>0.72599999999999998</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -4633,7 +4566,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1">
-        <v>0.45200000000000001</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
@@ -4677,7 +4610,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1">
-        <v>0.48599999999999999</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
@@ -4721,7 +4654,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1">
-        <v>0.53500000000000003</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
@@ -4765,7 +4698,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1">
-        <v>0.60399999999999998</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
@@ -4809,7 +4742,7 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1">
-        <v>0.59799999999999998</v>
+        <v>0.62</v>
       </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
@@ -4853,7 +4786,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1">
-        <v>0.62</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
@@ -4897,7 +4830,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1">
-        <v>0.66700000000000004</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -4940,9 +4873,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="1">
-        <v>0.60099999999999998</v>
-      </c>
+      <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -5146,7 +5077,9 @@
     <row r="79" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="C79" s="1">
+        <v>1.006</v>
+      </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -5154,8 +5087,12 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
+      <c r="K79" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="L79" s="1">
+        <v>1.4970000000000001</v>
+      </c>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -5189,7 +5126,7 @@
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1">
-        <v>1.006</v>
+        <v>1.157</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -5199,10 +5136,10 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1">
-        <v>0.65300000000000002</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="L80" s="1">
-        <v>1.4970000000000001</v>
+        <v>1.5609999999999999</v>
       </c>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
@@ -5237,7 +5174,7 @@
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1">
-        <v>1.157</v>
+        <v>1.2769999999999999</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -5250,7 +5187,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="L81" s="1">
-        <v>1.5609999999999999</v>
+        <v>1.8140000000000001</v>
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
@@ -5285,7 +5222,7 @@
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1">
-        <v>1.2769999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -5295,10 +5232,10 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1">
-        <v>0.56999999999999995</v>
+        <v>0.68</v>
       </c>
       <c r="L82" s="1">
-        <v>1.8140000000000001</v>
+        <v>1.38</v>
       </c>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
@@ -5333,7 +5270,7 @@
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1">
-        <v>1.0900000000000001</v>
+        <v>1.181</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -5343,10 +5280,10 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1">
-        <v>0.68</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="L83" s="1">
-        <v>1.38</v>
+        <v>1.603</v>
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
@@ -5381,7 +5318,7 @@
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1">
-        <v>1.181</v>
+        <v>1.27</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -5391,10 +5328,10 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1">
-        <v>0.55400000000000005</v>
+        <v>0.625</v>
       </c>
       <c r="L84" s="1">
-        <v>1.603</v>
+        <v>1.5309999999999999</v>
       </c>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
@@ -5429,7 +5366,7 @@
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1">
-        <v>1.27</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -5439,10 +5376,10 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1">
-        <v>0.625</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="L85" s="1">
-        <v>1.5309999999999999</v>
+        <v>2.0619999999999998</v>
       </c>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
@@ -5477,7 +5414,7 @@
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1">
-        <v>1.1639999999999999</v>
+        <v>1.0229999999999999</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -5487,10 +5424,10 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1">
-        <v>0.61799999999999999</v>
+        <v>0.622</v>
       </c>
       <c r="L86" s="1">
-        <v>2.0619999999999998</v>
+        <v>1.591</v>
       </c>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
@@ -5525,7 +5462,7 @@
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1">
-        <v>1.0229999999999999</v>
+        <v>1.175</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -5535,10 +5472,10 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1">
-        <v>0.622</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="L87" s="1">
-        <v>1.591</v>
+        <v>1.7629999999999999</v>
       </c>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
@@ -5573,7 +5510,7 @@
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1">
-        <v>1.175</v>
+        <v>1.0489999999999999</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -5583,10 +5520,10 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1">
-        <v>0.59699999999999998</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="L88" s="1">
-        <v>1.7629999999999999</v>
+        <v>2</v>
       </c>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
@@ -5621,7 +5558,7 @@
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1">
-        <v>1.0489999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -5631,10 +5568,10 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1">
-        <v>0.59799999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="L89" s="1">
-        <v>2</v>
+        <v>1.472</v>
       </c>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
@@ -5668,9 +5605,7 @@
     <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="1">
-        <v>1.0029999999999999</v>
-      </c>
+      <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -5682,7 +5617,7 @@
         <v>0.625</v>
       </c>
       <c r="L90" s="1">
-        <v>1.472</v>
+        <v>1.5569999999999999</v>
       </c>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
@@ -5725,10 +5660,10 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1">
-        <v>0.625</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="L91" s="1">
-        <v>1.5569999999999999</v>
+        <v>1.726</v>
       </c>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
@@ -5771,10 +5706,10 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1">
-        <v>0.55200000000000005</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="L92" s="1">
-        <v>1.726</v>
+        <v>1.619</v>
       </c>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
@@ -5817,10 +5752,10 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1">
-        <v>0.56499999999999995</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="L93" s="1">
-        <v>1.619</v>
+        <v>1.506</v>
       </c>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
@@ -5863,10 +5798,10 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1">
-        <v>0.60899999999999999</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="L94" s="1">
-        <v>1.506</v>
+        <v>1.4350000000000001</v>
       </c>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
@@ -5909,10 +5844,10 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
       <c r="K95" s="1">
-        <v>0.54900000000000004</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="L95" s="1">
-        <v>1.4350000000000001</v>
+        <v>1.3680000000000001</v>
       </c>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
@@ -5955,11 +5890,9 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
       <c r="K96" s="1">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="L96" s="1">
-        <v>1.3680000000000001</v>
-      </c>
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="L96" s="1"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
@@ -6001,7 +5934,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
       <c r="K97" s="1">
-        <v>0.59699999999999998</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
@@ -6044,9 +5977,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
-      <c r="K98" s="1">
-        <v>0.58599999999999997</v>
-      </c>
+      <c r="K98" s="1"/>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
@@ -6162,12 +6093,20 @@
       <c r="AN100" s="1"/>
     </row>
     <row r="101" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
+      <c r="A101" s="1">
+        <v>1.466</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1.899</v>
+      </c>
       <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="D101" s="1">
+        <v>1.0409999999999999</v>
+      </c>
       <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
+      <c r="F101" s="1">
+        <v>0.70599999999999996</v>
+      </c>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
@@ -6205,18 +6144,18 @@
     </row>
     <row r="102" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>1.466</v>
+        <v>1.401</v>
       </c>
       <c r="B102" s="1">
-        <v>1.899</v>
+        <v>1.5620000000000001</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1">
-        <v>1.0409999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1">
-        <v>0.70599999999999996</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
@@ -6255,18 +6194,18 @@
     </row>
     <row r="103" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>1.401</v>
+        <v>1.4590000000000001</v>
       </c>
       <c r="B103" s="1">
-        <v>1.5620000000000001</v>
+        <v>1.7410000000000001</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1">
-        <v>1.1000000000000001</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1">
-        <v>0.61399999999999999</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
@@ -6305,18 +6244,18 @@
     </row>
     <row r="104" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>1.4590000000000001</v>
+        <v>1.4359999999999999</v>
       </c>
       <c r="B104" s="1">
-        <v>1.7410000000000001</v>
+        <v>1.758</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1">
-        <v>0.90200000000000002</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1">
-        <v>0.65500000000000003</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
@@ -6355,18 +6294,18 @@
     </row>
     <row r="105" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>1.4359999999999999</v>
+        <v>1.7210000000000001</v>
       </c>
       <c r="B105" s="1">
-        <v>1.758</v>
+        <v>1.6830000000000001</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1">
-        <v>0.82499999999999996</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1">
-        <v>0.63200000000000001</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -6405,18 +6344,18 @@
     </row>
     <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>1.7210000000000001</v>
+        <v>1.4419999999999999</v>
       </c>
       <c r="B106" s="1">
-        <v>1.6830000000000001</v>
+        <v>2.1859999999999999</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1">
-        <v>0.91800000000000004</v>
+        <v>1.4430000000000001</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1">
-        <v>0.60899999999999999</v>
+        <v>0.62</v>
       </c>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
@@ -6455,18 +6394,18 @@
     </row>
     <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>1.4419999999999999</v>
+        <v>1.8720000000000001</v>
       </c>
       <c r="B107" s="1">
-        <v>2.1859999999999999</v>
+        <v>1.345</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1">
-        <v>1.4430000000000001</v>
+        <v>1.196</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1">
-        <v>0.62</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
@@ -6505,18 +6444,18 @@
     </row>
     <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>1.8720000000000001</v>
+        <v>1.6559999999999999</v>
       </c>
       <c r="B108" s="1">
-        <v>1.345</v>
+        <v>1.2230000000000001</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1">
-        <v>1.196</v>
+        <v>0.85</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1">
-        <v>0.59499999999999997</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
@@ -6555,19 +6494,15 @@
     </row>
     <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>1.6559999999999999</v>
-      </c>
-      <c r="B109" s="1">
-        <v>1.2230000000000001</v>
-      </c>
+        <v>1.47</v>
+      </c>
+      <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1">
-        <v>0.85</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="E109" s="1"/>
-      <c r="F109" s="1">
-        <v>0.67100000000000004</v>
-      </c>
+      <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
@@ -6605,12 +6540,12 @@
     </row>
     <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>1.47</v>
+        <v>1.6970000000000001</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1">
-        <v>1.0580000000000001</v>
+        <v>1.6839999999999999</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -6651,12 +6586,12 @@
     </row>
     <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>1.6970000000000001</v>
+        <v>1.484</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1">
-        <v>1.6839999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -6697,12 +6632,12 @@
     </row>
     <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>1.484</v>
+        <v>1.353</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1">
-        <v>0.98799999999999999</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -6742,13 +6677,11 @@
       <c r="AN112" s="1"/>
     </row>
     <row r="113" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A113" s="1">
-        <v>1.353</v>
-      </c>
+      <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1">
-        <v>0.96899999999999997</v>
+        <v>1.04</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -6787,50 +6720,6 @@
       <c r="AM113" s="1"/>
       <c r="AN113" s="1"/>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1">
-        <v>1.04</v>
-      </c>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="1"/>
-      <c r="J114" s="1"/>
-      <c r="K114" s="1"/>
-      <c r="L114" s="1"/>
-      <c r="M114" s="1"/>
-      <c r="N114" s="1"/>
-      <c r="O114" s="1"/>
-      <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
-      <c r="R114" s="1"/>
-      <c r="S114" s="1"/>
-      <c r="T114" s="1"/>
-      <c r="U114" s="1"/>
-      <c r="V114" s="1"/>
-      <c r="W114" s="1"/>
-      <c r="X114" s="1"/>
-      <c r="Y114" s="1"/>
-      <c r="Z114" s="1"/>
-      <c r="AA114" s="1"/>
-      <c r="AB114" s="1"/>
-      <c r="AC114" s="1"/>
-      <c r="AD114" s="1"/>
-      <c r="AE114" s="1"/>
-      <c r="AF114" s="1"/>
-      <c r="AG114" s="1"/>
-      <c r="AH114" s="1"/>
-      <c r="AI114" s="1"/>
-      <c r="AJ114" s="1"/>
-      <c r="AK114" s="1"/>
-      <c r="AL114" s="1"/>
-      <c r="AM114" s="1"/>
-      <c r="AN114" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mboat7-2 and EndophilinA1 added
</commit_message>
<xml_diff>
--- a/SourceData/NEES.xlsx
+++ b/SourceData/NEES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6B654C-7934-774B-BFC6-918031F2C3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F9EE5-1E2A-9F4C-B490-07EB6D44AF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="1040" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>TMEM214</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Mdomain</t>
+  </si>
+  <si>
+    <t>Endophilin A1</t>
   </si>
 </sst>
 </file>
@@ -536,15 +539,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC4DC55-F2F9-5F4B-B79C-9C9FBA074888}">
-  <dimension ref="A1:AN113"/>
+  <dimension ref="A1:AO113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+      <selection activeCell="AF21" sqref="AF21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -665,8 +668,11 @@
       <c r="AN1" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.86499999999999999</v>
       </c>
@@ -740,7 +746,9 @@
       <c r="AE2" s="1">
         <v>0.48199999999999998</v>
       </c>
-      <c r="AF2" s="1"/>
+      <c r="AF2" s="1">
+        <v>0.54600000000000004</v>
+      </c>
       <c r="AG2" s="1">
         <v>0.41</v>
       </c>
@@ -765,8 +773,11 @@
       <c r="AN2" s="1">
         <v>0.45200000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO2" s="1">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.99</v>
       </c>
@@ -840,7 +851,9 @@
       <c r="AE3" s="1">
         <v>0.40300000000000002</v>
       </c>
-      <c r="AF3" s="1"/>
+      <c r="AF3" s="1">
+        <v>0.55300000000000005</v>
+      </c>
       <c r="AG3" s="1">
         <v>0.40100000000000002</v>
       </c>
@@ -865,8 +878,11 @@
       <c r="AN3" s="1">
         <v>0.51900000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO3" s="1">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1.069</v>
       </c>
@@ -940,7 +956,9 @@
       <c r="AE4" s="1">
         <v>0.46899999999999997</v>
       </c>
-      <c r="AF4" s="1"/>
+      <c r="AF4" s="1">
+        <v>0.56200000000000006</v>
+      </c>
       <c r="AG4" s="1">
         <v>0.47799999999999998</v>
       </c>
@@ -965,8 +983,11 @@
       <c r="AN4" s="1">
         <v>0.40899999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO4" s="1">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1.1579999999999999</v>
       </c>
@@ -1040,7 +1061,9 @@
       <c r="AE5" s="1">
         <v>0.501</v>
       </c>
-      <c r="AF5" s="1"/>
+      <c r="AF5" s="1">
+        <v>0.51300000000000001</v>
+      </c>
       <c r="AG5" s="1">
         <v>0.39</v>
       </c>
@@ -1065,8 +1088,11 @@
       <c r="AN5" s="1">
         <v>0.41099999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO5" s="1">
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1.0940000000000001</v>
       </c>
@@ -1140,7 +1166,9 @@
       <c r="AE6" s="1">
         <v>0.443</v>
       </c>
-      <c r="AF6" s="1"/>
+      <c r="AF6" s="1">
+        <v>0.501</v>
+      </c>
       <c r="AG6" s="1">
         <v>0.47899999999999998</v>
       </c>
@@ -1165,8 +1193,11 @@
       <c r="AN6" s="1">
         <v>0.44900000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO6" s="1">
+        <v>0.436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1.1499999999999999</v>
       </c>
@@ -1240,7 +1271,9 @@
       <c r="AE7" s="1">
         <v>0.48</v>
       </c>
-      <c r="AF7" s="1"/>
+      <c r="AF7" s="1">
+        <v>0.66400000000000003</v>
+      </c>
       <c r="AG7" s="1">
         <v>0.436</v>
       </c>
@@ -1265,8 +1298,11 @@
       <c r="AN7" s="1">
         <v>0.45400000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO7" s="1">
+        <v>0.38900000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.123</v>
       </c>
@@ -1340,7 +1376,9 @@
       <c r="AE8" s="1">
         <v>0.40200000000000002</v>
       </c>
-      <c r="AF8" s="1"/>
+      <c r="AF8" s="1">
+        <v>0.66400000000000003</v>
+      </c>
       <c r="AG8" s="1">
         <v>0.45</v>
       </c>
@@ -1365,8 +1403,11 @@
       <c r="AN8" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO8" s="1">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.103</v>
       </c>
@@ -1440,7 +1481,9 @@
       <c r="AE9" s="1">
         <v>0.45500000000000002</v>
       </c>
-      <c r="AF9" s="1"/>
+      <c r="AF9" s="1">
+        <v>0.66900000000000004</v>
+      </c>
       <c r="AG9" s="1">
         <v>0.53400000000000003</v>
       </c>
@@ -1465,8 +1508,11 @@
       <c r="AN9" s="1">
         <v>0.48399999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO9" s="1">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.99399999999999999</v>
       </c>
@@ -1540,7 +1586,9 @@
       <c r="AE10" s="1">
         <v>0.43</v>
       </c>
-      <c r="AF10" s="1"/>
+      <c r="AF10" s="1">
+        <v>0.51</v>
+      </c>
       <c r="AG10" s="1">
         <v>0.48899999999999999</v>
       </c>
@@ -1565,8 +1613,11 @@
       <c r="AN10" s="1">
         <v>0.41599999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO10" s="1">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1.133</v>
       </c>
@@ -1638,7 +1689,9 @@
       <c r="AE11" s="1">
         <v>0.36099999999999999</v>
       </c>
-      <c r="AF11" s="1"/>
+      <c r="AF11" s="1">
+        <v>0.51700000000000002</v>
+      </c>
       <c r="AG11" s="1">
         <v>0.55200000000000005</v>
       </c>
@@ -1663,8 +1716,11 @@
       <c r="AN11" s="1">
         <v>0.53300000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO11" s="1">
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1.1879999999999999</v>
       </c>
@@ -1732,7 +1788,9 @@
       <c r="AE12" s="1">
         <v>0.40400000000000003</v>
       </c>
-      <c r="AF12" s="1"/>
+      <c r="AF12" s="1">
+        <v>0.505</v>
+      </c>
       <c r="AG12" s="1">
         <v>0.47699999999999998</v>
       </c>
@@ -1755,8 +1813,11 @@
       <c r="AN12" s="1">
         <v>0.503</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO12" s="1">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1.155</v>
       </c>
@@ -1816,7 +1877,9 @@
       </c>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
+      <c r="AF13" s="1">
+        <v>0.48699999999999999</v>
+      </c>
       <c r="AG13" s="1">
         <v>0.441</v>
       </c>
@@ -1837,8 +1900,11 @@
       <c r="AN13" s="1">
         <v>0.42399999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO13" s="1">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1.127</v>
       </c>
@@ -1892,7 +1958,9 @@
       </c>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
+      <c r="AF14" s="1">
+        <v>0.501</v>
+      </c>
       <c r="AG14" s="1">
         <v>0.54400000000000004</v>
       </c>
@@ -1911,8 +1979,11 @@
       </c>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO14" s="1">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1.1419999999999999</v>
       </c>
@@ -1966,7 +2037,9 @@
       </c>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
+      <c r="AF15" s="1">
+        <v>0.66500000000000004</v>
+      </c>
       <c r="AG15" s="1">
         <v>0.47399999999999998</v>
       </c>
@@ -1981,8 +2054,11 @@
       </c>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO15" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1.2290000000000001</v>
       </c>
@@ -2032,7 +2108,9 @@
       </c>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
+      <c r="AF16" s="1">
+        <v>0.54</v>
+      </c>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -2043,6 +2121,9 @@
       </c>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
+      <c r="AO16" s="1">
+        <v>0.47599999999999998</v>
+      </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -2088,7 +2169,9 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
+      <c r="AF17" s="1">
+        <v>0.42799999999999999</v>
+      </c>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
@@ -2144,7 +2227,9 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
+      <c r="AF18" s="1">
+        <v>0.63900000000000001</v>
+      </c>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2192,7 +2277,9 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
+      <c r="AF19" s="1">
+        <v>0.69099999999999995</v>
+      </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2240,7 +2327,9 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
-      <c r="AF20" s="1"/>
+      <c r="AF20" s="1">
+        <v>0.41599999999999998</v>
+      </c>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -2296,7 +2385,9 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
-      <c r="AF21" s="1"/>
+      <c r="AF21" s="1">
+        <v>0.53</v>
+      </c>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
@@ -2350,7 +2441,6 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
-      <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
@@ -2506,7 +2596,6 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>

</xml_diff>

<commit_message>
EndophilinA1 added and ddF for characterized AHs added
</commit_message>
<xml_diff>
--- a/SourceData/NEES.xlsx
+++ b/SourceData/NEES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F9EE5-1E2A-9F4C-B490-07EB6D44AF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9EA68A-CE4F-D64D-B620-B802935B0658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="1040" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
   </bookViews>
@@ -158,7 +158,7 @@
     <t>Mdomain</t>
   </si>
   <si>
-    <t>Endophilin A1</t>
+    <t>EndophilinA1</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC4DC55-F2F9-5F4B-B79C-9C9FBA074888}">
   <dimension ref="A1:AO113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AF21" sqref="AF21"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Corrected NEES by removing remnant of old NEES
</commit_message>
<xml_diff>
--- a/SourceData/NEES.xlsx
+++ b/SourceData/NEES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9311FD9-5193-AC4C-A54A-53B872427911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F324AE2-628C-F141-B175-8434F3B2C792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1040" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
+    <workbookView xWindow="2460" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC4DC55-F2F9-5F4B-B79C-9C9FBA074888}">
   <dimension ref="A1:AU113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1:AU13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M137" sqref="M137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2244,6 +2244,8 @@
         <v>0.58099999999999996</v>
       </c>
       <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -2323,6 +2325,8 @@
         <v>0.61199999999999999</v>
       </c>
       <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -2396,8 +2400,10 @@
         <v>0.66</v>
       </c>
       <c r="AS16" s="1"/>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2459,8 +2465,10 @@
       <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
       <c r="AS17" s="1"/>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2518,8 +2526,10 @@
       <c r="AQ18" s="1"/>
       <c r="AR18" s="1"/>
       <c r="AS18" s="1"/>
-    </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2577,8 +2587,10 @@
       <c r="AQ19" s="1"/>
       <c r="AR19" s="1"/>
       <c r="AS19" s="1"/>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2632,8 +2644,10 @@
       <c r="AQ20" s="1"/>
       <c r="AR20" s="1"/>
       <c r="AS20" s="1"/>
-    </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>1.944</v>
@@ -2693,8 +2707,10 @@
       <c r="AQ21" s="1"/>
       <c r="AR21" s="1"/>
       <c r="AS21" s="1"/>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>1.86</v>
@@ -2750,8 +2766,10 @@
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
       <c r="AS22" s="1"/>
-    </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>2.0449999999999999</v>
@@ -2803,8 +2821,10 @@
       <c r="AQ23" s="1"/>
       <c r="AR23" s="1"/>
       <c r="AS23" s="1"/>
-    </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT23" s="1"/>
+      <c r="AU23" s="1"/>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>2.2410000000000001</v>
@@ -2856,8 +2876,10 @@
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1"/>
       <c r="AS24" s="1"/>
-    </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>2.4119999999999999</v>
@@ -2909,8 +2931,10 @@
       <c r="AQ25" s="1"/>
       <c r="AR25" s="1"/>
       <c r="AS25" s="1"/>
-    </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>2.319</v>
@@ -2962,8 +2986,10 @@
       <c r="AQ26" s="1"/>
       <c r="AR26" s="1"/>
       <c r="AS26" s="1"/>
-    </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1">
         <v>1.88</v>
@@ -3013,8 +3039,10 @@
       <c r="AQ27" s="1"/>
       <c r="AR27" s="1"/>
       <c r="AS27" s="1"/>
-    </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <v>1.986</v>
@@ -3064,8 +3092,10 @@
       <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
       <c r="AS28" s="1"/>
-    </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <v>1.091</v>
@@ -3115,8 +3145,10 @@
       <c r="AQ29" s="1"/>
       <c r="AR29" s="1"/>
       <c r="AS29" s="1"/>
-    </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <v>2.1120000000000001</v>
@@ -3166,8 +3198,10 @@
       <c r="AQ30" s="1"/>
       <c r="AR30" s="1"/>
       <c r="AS30" s="1"/>
-    </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT30" s="1"/>
+      <c r="AU30" s="1"/>
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3213,8 +3247,10 @@
       <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
       <c r="AS31" s="1"/>
-    </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT31" s="1"/>
+      <c r="AU31" s="1"/>
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3260,8 +3296,10 @@
       <c r="AQ32" s="1"/>
       <c r="AR32" s="1"/>
       <c r="AS32" s="1"/>
-    </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT32" s="1"/>
+      <c r="AU32" s="1"/>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3307,8 +3345,10 @@
       <c r="AQ33" s="1"/>
       <c r="AR33" s="1"/>
       <c r="AS33" s="1"/>
-    </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT33" s="1"/>
+      <c r="AU33" s="1"/>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3354,8 +3394,10 @@
       <c r="AQ34" s="1"/>
       <c r="AR34" s="1"/>
       <c r="AS34" s="1"/>
-    </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT34" s="1"/>
+      <c r="AU34" s="1"/>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3401,8 +3443,10 @@
       <c r="AQ35" s="1"/>
       <c r="AR35" s="1"/>
       <c r="AS35" s="1"/>
-    </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT35" s="1"/>
+      <c r="AU35" s="1"/>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3448,8 +3492,10 @@
       <c r="AQ36" s="1"/>
       <c r="AR36" s="1"/>
       <c r="AS36" s="1"/>
-    </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT36" s="1"/>
+      <c r="AU36" s="1"/>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
@@ -3503,8 +3549,10 @@
       <c r="AQ37" s="1"/>
       <c r="AR37" s="1"/>
       <c r="AS37" s="1"/>
-    </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT37" s="1"/>
+      <c r="AU37" s="1"/>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1">
@@ -3558,8 +3606,10 @@
       <c r="AQ38" s="1"/>
       <c r="AR38" s="1"/>
       <c r="AS38" s="1"/>
-    </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT38" s="1"/>
+      <c r="AU38" s="1"/>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1">
@@ -3613,8 +3663,10 @@
       <c r="AQ39" s="1"/>
       <c r="AR39" s="1"/>
       <c r="AS39" s="1"/>
-    </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT39" s="1"/>
+      <c r="AU39" s="1"/>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1">
@@ -3668,8 +3720,10 @@
       <c r="AQ40" s="1"/>
       <c r="AR40" s="1"/>
       <c r="AS40" s="1"/>
-    </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT40" s="1"/>
+      <c r="AU40" s="1"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1">
@@ -3723,8 +3777,10 @@
       <c r="AQ41" s="1"/>
       <c r="AR41" s="1"/>
       <c r="AS41" s="1"/>
-    </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT41" s="1"/>
+      <c r="AU41" s="1"/>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1">
@@ -3778,8 +3834,10 @@
       <c r="AQ42" s="1"/>
       <c r="AR42" s="1"/>
       <c r="AS42" s="1"/>
-    </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT42" s="1"/>
+      <c r="AU42" s="1"/>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1">
@@ -3833,8 +3891,10 @@
       <c r="AQ43" s="1"/>
       <c r="AR43" s="1"/>
       <c r="AS43" s="1"/>
-    </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT43" s="1"/>
+      <c r="AU43" s="1"/>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1">
@@ -3888,8 +3948,10 @@
       <c r="AQ44" s="1"/>
       <c r="AR44" s="1"/>
       <c r="AS44" s="1"/>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT44" s="1"/>
+      <c r="AU44" s="1"/>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1">
@@ -3943,8 +4005,10 @@
       <c r="AQ45" s="1"/>
       <c r="AR45" s="1"/>
       <c r="AS45" s="1"/>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT45" s="1"/>
+      <c r="AU45" s="1"/>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1">
@@ -3998,8 +4062,10 @@
       <c r="AQ46" s="1"/>
       <c r="AR46" s="1"/>
       <c r="AS46" s="1"/>
-    </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT46" s="1"/>
+      <c r="AU46" s="1"/>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1">
@@ -4053,8 +4119,10 @@
       <c r="AQ47" s="1"/>
       <c r="AR47" s="1"/>
       <c r="AS47" s="1"/>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT47" s="1"/>
+      <c r="AU47" s="1"/>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1">
@@ -4106,8 +4174,10 @@
       <c r="AQ48" s="1"/>
       <c r="AR48" s="1"/>
       <c r="AS48" s="1"/>
-    </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT48" s="1"/>
+      <c r="AU48" s="1"/>
+    </row>
+    <row r="49" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1">
@@ -4159,8 +4229,10 @@
       <c r="AQ49" s="1"/>
       <c r="AR49" s="1"/>
       <c r="AS49" s="1"/>
-    </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT49" s="1"/>
+      <c r="AU49" s="1"/>
+    </row>
+    <row r="50" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4210,8 +4282,10 @@
       <c r="AQ50" s="1"/>
       <c r="AR50" s="1"/>
       <c r="AS50" s="1"/>
-    </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT50" s="1"/>
+      <c r="AU50" s="1"/>
+    </row>
+    <row r="51" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -4259,8 +4333,10 @@
       <c r="AQ51" s="1"/>
       <c r="AR51" s="1"/>
       <c r="AS51" s="1"/>
-    </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT51" s="1"/>
+      <c r="AU51" s="1"/>
+    </row>
+    <row r="52" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -4308,8 +4384,10 @@
       <c r="AQ52" s="1"/>
       <c r="AR52" s="1"/>
       <c r="AS52" s="1"/>
-    </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT52" s="1"/>
+      <c r="AU52" s="1"/>
+    </row>
+    <row r="53" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -4357,8 +4435,10 @@
       <c r="AQ53" s="1"/>
       <c r="AR53" s="1"/>
       <c r="AS53" s="1"/>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT53" s="1"/>
+      <c r="AU53" s="1"/>
+    </row>
+    <row r="54" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -4406,8 +4486,10 @@
       <c r="AQ54" s="1"/>
       <c r="AR54" s="1"/>
       <c r="AS54" s="1"/>
-    </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT54" s="1"/>
+      <c r="AU54" s="1"/>
+    </row>
+    <row r="55" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -4455,8 +4537,10 @@
       <c r="AQ55" s="1"/>
       <c r="AR55" s="1"/>
       <c r="AS55" s="1"/>
-    </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT55" s="1"/>
+      <c r="AU55" s="1"/>
+    </row>
+    <row r="56" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -4504,8 +4588,10 @@
       <c r="AQ56" s="1"/>
       <c r="AR56" s="1"/>
       <c r="AS56" s="1"/>
-    </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT56" s="1"/>
+      <c r="AU56" s="1"/>
+    </row>
+    <row r="57" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -4551,8 +4637,10 @@
       <c r="AQ57" s="1"/>
       <c r="AR57" s="1"/>
       <c r="AS57" s="1"/>
-    </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT57" s="1"/>
+      <c r="AU57" s="1"/>
+    </row>
+    <row r="58" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4598,8 +4686,10 @@
       <c r="AQ58" s="1"/>
       <c r="AR58" s="1"/>
       <c r="AS58" s="1"/>
-    </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT58" s="1"/>
+      <c r="AU58" s="1"/>
+    </row>
+    <row r="59" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4645,8 +4735,10 @@
       <c r="AQ59" s="1"/>
       <c r="AR59" s="1"/>
       <c r="AS59" s="1"/>
-    </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT59" s="1"/>
+      <c r="AU59" s="1"/>
+    </row>
+    <row r="60" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4694,8 +4786,10 @@
       <c r="AQ60" s="1"/>
       <c r="AR60" s="1"/>
       <c r="AS60" s="1"/>
-    </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT60" s="1"/>
+      <c r="AU60" s="1"/>
+    </row>
+    <row r="61" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4743,8 +4837,10 @@
       <c r="AQ61" s="1"/>
       <c r="AR61" s="1"/>
       <c r="AS61" s="1"/>
-    </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT61" s="1"/>
+      <c r="AU61" s="1"/>
+    </row>
+    <row r="62" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4792,8 +4888,10 @@
       <c r="AQ62" s="1"/>
       <c r="AR62" s="1"/>
       <c r="AS62" s="1"/>
-    </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT62" s="1"/>
+      <c r="AU62" s="1"/>
+    </row>
+    <row r="63" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4841,8 +4939,10 @@
       <c r="AQ63" s="1"/>
       <c r="AR63" s="1"/>
       <c r="AS63" s="1"/>
-    </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT63" s="1"/>
+      <c r="AU63" s="1"/>
+    </row>
+    <row r="64" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4890,8 +4990,10 @@
       <c r="AQ64" s="1"/>
       <c r="AR64" s="1"/>
       <c r="AS64" s="1"/>
-    </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT64" s="1"/>
+      <c r="AU64" s="1"/>
+    </row>
+    <row r="65" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4939,8 +5041,10 @@
       <c r="AQ65" s="1"/>
       <c r="AR65" s="1"/>
       <c r="AS65" s="1"/>
-    </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT65" s="1"/>
+      <c r="AU65" s="1"/>
+    </row>
+    <row r="66" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4988,8 +5092,10 @@
       <c r="AQ66" s="1"/>
       <c r="AR66" s="1"/>
       <c r="AS66" s="1"/>
-    </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT66" s="1"/>
+      <c r="AU66" s="1"/>
+    </row>
+    <row r="67" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -5037,8 +5143,10 @@
       <c r="AQ67" s="1"/>
       <c r="AR67" s="1"/>
       <c r="AS67" s="1"/>
-    </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT67" s="1"/>
+      <c r="AU67" s="1"/>
+    </row>
+    <row r="68" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -5086,8 +5194,10 @@
       <c r="AQ68" s="1"/>
       <c r="AR68" s="1"/>
       <c r="AS68" s="1"/>
-    </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT68" s="1"/>
+      <c r="AU68" s="1"/>
+    </row>
+    <row r="69" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -5135,8 +5245,10 @@
       <c r="AQ69" s="1"/>
       <c r="AR69" s="1"/>
       <c r="AS69" s="1"/>
-    </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT69" s="1"/>
+      <c r="AU69" s="1"/>
+    </row>
+    <row r="70" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -5184,8 +5296,10 @@
       <c r="AQ70" s="1"/>
       <c r="AR70" s="1"/>
       <c r="AS70" s="1"/>
-    </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT70" s="1"/>
+      <c r="AU70" s="1"/>
+    </row>
+    <row r="71" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -5233,8 +5347,10 @@
       <c r="AQ71" s="1"/>
       <c r="AR71" s="1"/>
       <c r="AS71" s="1"/>
-    </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT71" s="1"/>
+      <c r="AU71" s="1"/>
+    </row>
+    <row r="72" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -5282,8 +5398,10 @@
       <c r="AQ72" s="1"/>
       <c r="AR72" s="1"/>
       <c r="AS72" s="1"/>
-    </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT72" s="1"/>
+      <c r="AU72" s="1"/>
+    </row>
+    <row r="73" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -5331,8 +5449,10 @@
       <c r="AQ73" s="1"/>
       <c r="AR73" s="1"/>
       <c r="AS73" s="1"/>
-    </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT73" s="1"/>
+      <c r="AU73" s="1"/>
+    </row>
+    <row r="74" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -5379,7 +5499,7 @@
       <c r="AR74" s="1"/>
       <c r="AS74" s="1"/>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -5426,7 +5546,7 @@
       <c r="AR75" s="1"/>
       <c r="AS75" s="1"/>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -5473,7 +5593,7 @@
       <c r="AR76" s="1"/>
       <c r="AS76" s="1"/>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -5520,7 +5640,7 @@
       <c r="AR77" s="1"/>
       <c r="AS77" s="1"/>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -5562,12 +5682,10 @@
       <c r="AM78" s="1"/>
       <c r="AN78" s="1"/>
     </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="1">
-        <v>1.006</v>
-      </c>
+      <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -5575,12 +5693,8 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
-      <c r="K79" s="1">
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="L79" s="1">
-        <v>1.4970000000000001</v>
-      </c>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -5610,12 +5724,10 @@
       <c r="AM79" s="1"/>
       <c r="AN79" s="1"/>
     </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="1">
-        <v>1.157</v>
-      </c>
+      <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -5623,12 +5735,8 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-      <c r="K80" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L80" s="1">
-        <v>1.5609999999999999</v>
-      </c>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -5661,9 +5769,7 @@
     <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="1">
-        <v>1.2769999999999999</v>
-      </c>
+      <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -5671,12 +5777,8 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
-      <c r="K81" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L81" s="1">
-        <v>1.8140000000000001</v>
-      </c>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -5709,9 +5811,7 @@
     <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="1">
-        <v>1.0900000000000001</v>
-      </c>
+      <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -5719,12 +5819,8 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
-      <c r="K82" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="L82" s="1">
-        <v>1.38</v>
-      </c>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
@@ -5757,9 +5853,7 @@
     <row r="83" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="C83" s="1">
-        <v>1.181</v>
-      </c>
+      <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -5767,12 +5861,8 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
-      <c r="K83" s="1">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="L83" s="1">
-        <v>1.603</v>
-      </c>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
@@ -5805,9 +5895,7 @@
     <row r="84" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="1">
-        <v>1.27</v>
-      </c>
+      <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -5815,12 +5903,8 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
-      <c r="K84" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="L84" s="1">
-        <v>1.5309999999999999</v>
-      </c>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
@@ -5853,9 +5937,7 @@
     <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
-        <v>1.1639999999999999</v>
-      </c>
+      <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -5863,12 +5945,8 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
-      <c r="K85" s="1">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="L85" s="1">
-        <v>2.0619999999999998</v>
-      </c>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
@@ -5901,9 +5979,7 @@
     <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="1">
-        <v>1.0229999999999999</v>
-      </c>
+      <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -5911,12 +5987,8 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
-      <c r="K86" s="1">
-        <v>0.622</v>
-      </c>
-      <c r="L86" s="1">
-        <v>1.591</v>
-      </c>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
@@ -5949,9 +6021,7 @@
     <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="1">
-        <v>1.175</v>
-      </c>
+      <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -5959,12 +6029,8 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
-      <c r="K87" s="1">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="L87" s="1">
-        <v>1.7629999999999999</v>
-      </c>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
@@ -5997,9 +6063,7 @@
     <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="C88" s="1">
-        <v>1.0489999999999999</v>
-      </c>
+      <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -6007,12 +6071,8 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
-      <c r="K88" s="1">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="L88" s="1">
-        <v>2</v>
-      </c>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
@@ -6045,9 +6105,7 @@
     <row r="89" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="1">
-        <v>1.0029999999999999</v>
-      </c>
+      <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -6055,12 +6113,8 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
-      <c r="K89" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="L89" s="1">
-        <v>1.472</v>
-      </c>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
@@ -6101,12 +6155,8 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
-      <c r="K90" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="L90" s="1">
-        <v>1.5569999999999999</v>
-      </c>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
@@ -6147,12 +6197,8 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
-      <c r="K91" s="1">
-        <v>0.55200000000000005</v>
-      </c>
-      <c r="L91" s="1">
-        <v>1.726</v>
-      </c>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
@@ -6193,12 +6239,8 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
-      <c r="K92" s="1">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="L92" s="1">
-        <v>1.619</v>
-      </c>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -6239,12 +6281,8 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
-      <c r="K93" s="1">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="L93" s="1">
-        <v>1.506</v>
-      </c>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -6285,12 +6323,8 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
-      <c r="K94" s="1">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="L94" s="1">
-        <v>1.4350000000000001</v>
-      </c>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -6331,12 +6365,8 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
-      <c r="K95" s="1">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="L95" s="1">
-        <v>1.3680000000000001</v>
-      </c>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -6377,9 +6407,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
-      <c r="K96" s="1">
-        <v>0.59699999999999998</v>
-      </c>
+      <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
@@ -6421,9 +6449,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
-      <c r="K97" s="1">
-        <v>0.58599999999999997</v>
-      </c>
+      <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
@@ -6581,20 +6607,12 @@
       <c r="AN100" s="1"/>
     </row>
     <row r="101" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
-        <v>1.466</v>
-      </c>
-      <c r="B101" s="1">
-        <v>1.899</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
       <c r="C101" s="1"/>
-      <c r="D101" s="1">
-        <v>1.0409999999999999</v>
-      </c>
+      <c r="D101" s="1"/>
       <c r="E101" s="1"/>
-      <c r="F101" s="1">
-        <v>0.70599999999999996</v>
-      </c>
+      <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
@@ -6631,20 +6649,12 @@
       <c r="AN101" s="1"/>
     </row>
     <row r="102" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
-        <v>1.401</v>
-      </c>
-      <c r="B102" s="1">
-        <v>1.5620000000000001</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
       <c r="C102" s="1"/>
-      <c r="D102" s="1">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="1">
-        <v>0.61399999999999999</v>
-      </c>
+      <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
@@ -6681,20 +6691,12 @@
       <c r="AN102" s="1"/>
     </row>
     <row r="103" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
-        <v>1.4590000000000001</v>
-      </c>
-      <c r="B103" s="1">
-        <v>1.7410000000000001</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
       <c r="C103" s="1"/>
-      <c r="D103" s="1">
-        <v>0.90200000000000002</v>
-      </c>
+      <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="1">
-        <v>0.65500000000000003</v>
-      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
@@ -6731,20 +6733,12 @@
       <c r="AN103" s="1"/>
     </row>
     <row r="104" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
-        <v>1.4359999999999999</v>
-      </c>
-      <c r="B104" s="1">
-        <v>1.758</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
       <c r="C104" s="1"/>
-      <c r="D104" s="1">
-        <v>0.82499999999999996</v>
-      </c>
+      <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="1">
-        <v>0.63200000000000001</v>
-      </c>
+      <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
@@ -6781,20 +6775,12 @@
       <c r="AN104" s="1"/>
     </row>
     <row r="105" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
-        <v>1.7210000000000001</v>
-      </c>
-      <c r="B105" s="1">
-        <v>1.6830000000000001</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
       <c r="C105" s="1"/>
-      <c r="D105" s="1">
-        <v>0.91800000000000004</v>
-      </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="1">
-        <v>0.60899999999999999</v>
-      </c>
+      <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
@@ -6831,20 +6817,12 @@
       <c r="AN105" s="1"/>
     </row>
     <row r="106" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A106" s="1">
-        <v>1.4419999999999999</v>
-      </c>
-      <c r="B106" s="1">
-        <v>2.1859999999999999</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
       <c r="C106" s="1"/>
-      <c r="D106" s="1">
-        <v>1.4430000000000001</v>
-      </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="F106" s="1">
-        <v>0.62</v>
-      </c>
+      <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
@@ -6881,20 +6859,12 @@
       <c r="AN106" s="1"/>
     </row>
     <row r="107" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
-        <v>1.8720000000000001</v>
-      </c>
-      <c r="B107" s="1">
-        <v>1.345</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
       <c r="C107" s="1"/>
-      <c r="D107" s="1">
-        <v>1.196</v>
-      </c>
+      <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="1">
-        <v>0.59499999999999997</v>
-      </c>
+      <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
@@ -6931,20 +6901,12 @@
       <c r="AN107" s="1"/>
     </row>
     <row r="108" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
-        <v>1.6559999999999999</v>
-      </c>
-      <c r="B108" s="1">
-        <v>1.2230000000000001</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
       <c r="C108" s="1"/>
-      <c r="D108" s="1">
-        <v>0.85</v>
-      </c>
+      <c r="D108" s="1"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="1">
-        <v>0.67100000000000004</v>
-      </c>
+      <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
@@ -6981,14 +6943,10 @@
       <c r="AN108" s="1"/>
     </row>
     <row r="109" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
-        <v>1.47</v>
-      </c>
+      <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
-      <c r="D109" s="1">
-        <v>1.0580000000000001</v>
-      </c>
+      <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -7027,14 +6985,10 @@
       <c r="AN109" s="1"/>
     </row>
     <row r="110" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
-        <v>1.6970000000000001</v>
-      </c>
+      <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
-      <c r="D110" s="1">
-        <v>1.6839999999999999</v>
-      </c>
+      <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
@@ -7073,14 +7027,10 @@
       <c r="AN110" s="1"/>
     </row>
     <row r="111" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
-        <v>1.484</v>
-      </c>
+      <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
-      <c r="D111" s="1">
-        <v>0.98799999999999999</v>
-      </c>
+      <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
@@ -7119,14 +7069,10 @@
       <c r="AN111" s="1"/>
     </row>
     <row r="112" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A112" s="1">
-        <v>1.353</v>
-      </c>
+      <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-      <c r="D112" s="1">
-        <v>0.96899999999999997</v>
-      </c>
+      <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
@@ -7168,9 +7114,7 @@
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
-      <c r="D113" s="1">
-        <v>1.04</v>
-      </c>
+      <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>

</xml_diff>

<commit_message>
"No AH" to "NoAH" renamed
</commit_message>
<xml_diff>
--- a/SourceData/NEES.xlsx
+++ b/SourceData/NEES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F324AE2-628C-F141-B175-8434F3B2C792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFC4602-0A8D-DB44-9249-6FB3C536FBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>Lemd3</t>
   </si>
   <si>
-    <t>No AH</t>
-  </si>
-  <si>
     <t>SpoVM</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>Arf1</t>
+  </si>
+  <si>
+    <t>NoAH</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:AU113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M137" sqref="M137"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +597,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
@@ -690,22 +690,22 @@
         <v>32</v>
       </c>
       <c r="AP1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AQ1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correction No AH to NoAH
</commit_message>
<xml_diff>
--- a/SourceData/NEES.xlsx
+++ b/SourceData/NEES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCBF82-F83F-DE43-8BE9-9A8763DFE5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF1482-32D2-0948-9F72-3898C84F70F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{FB9891CF-C866-D04F-BECB-1E1FC697AD26}"/>
   </bookViews>
@@ -176,14 +176,14 @@
     <t>Arf1</t>
   </si>
   <si>
-    <t>No AH</t>
+    <t>NoAH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -559,13 +559,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC4DC55-F2F9-5F4B-B79C-9C9FBA074888}">
   <dimension ref="A1:AU113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="27" zoomScaleNormal="27" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -708,7 +708,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1.375</v>
       </c>
@@ -849,7 +849,7 @@
         <v>3.3439999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1.379</v>
       </c>
@@ -990,7 +990,7 @@
         <v>4.141</v>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1.1950000000000001</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>3.4620000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1.2490000000000001</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>3.528</v>
       </c>
     </row>
-    <row r="6" spans="1:47">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1.19</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>3.601</v>
       </c>
     </row>
-    <row r="7" spans="1:47">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1.2430000000000001</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:47">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.3580000000000001</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>3.3130000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:47">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.222</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>3.0529999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:47">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1.415</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>2.0579999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:47">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1.331</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>2.754</v>
       </c>
     </row>
-    <row r="12" spans="1:47">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
@@ -2231,7 +2231,7 @@
         <v>2.302</v>
       </c>
     </row>
-    <row r="13" spans="1:47">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="AU13" s="1"/>
     </row>
-    <row r="14" spans="1:47">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1.867</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>7.6029999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:47">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1.431</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>8.0380000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:47">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1.224</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>8.4139999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:47">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1.2929999999999999</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>2.0920000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:47">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>1.831</v>
@@ -2985,7 +2985,7 @@
         <v>4.2430000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1.7969999999999999</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:47">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1.2230000000000001</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>4.3689999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1.7050000000000001</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>5.1989999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1.59</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>6.2939999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1.1930000000000001</v>
       </c>
@@ -3588,7 +3588,7 @@
       <c r="AT23" s="1"/>
       <c r="AU23" s="1"/>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1.3080000000000001</v>
       </c>
@@ -3691,7 +3691,7 @@
       <c r="AT24" s="1"/>
       <c r="AU24" s="1"/>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1.84</v>
       </c>
@@ -3790,7 +3790,7 @@
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
     </row>
-    <row r="26" spans="1:47">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1">
@@ -3881,7 +3881,7 @@
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
     </row>
-    <row r="27" spans="1:47">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
@@ -3970,7 +3970,7 @@
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
     </row>
-    <row r="28" spans="1:47">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
@@ -4055,7 +4055,7 @@
       <c r="AT28" s="1"/>
       <c r="AU28" s="1"/>
     </row>
-    <row r="29" spans="1:47">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
@@ -4134,7 +4134,7 @@
       <c r="AT29" s="1"/>
       <c r="AU29" s="1"/>
     </row>
-    <row r="30" spans="1:47">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1">
@@ -4207,7 +4207,7 @@
       <c r="AT30" s="1"/>
       <c r="AU30" s="1"/>
     </row>
-    <row r="31" spans="1:47">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -4274,7 +4274,7 @@
       <c r="AT31" s="1"/>
       <c r="AU31" s="1"/>
     </row>
-    <row r="32" spans="1:47">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4339,7 +4339,7 @@
       <c r="AT32" s="1"/>
       <c r="AU32" s="1"/>
     </row>
-    <row r="33" spans="1:47">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -4404,7 +4404,7 @@
       <c r="AT33" s="1"/>
       <c r="AU33" s="1"/>
     </row>
-    <row r="34" spans="1:47">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -4465,7 +4465,7 @@
       <c r="AT34" s="1"/>
       <c r="AU34" s="1"/>
     </row>
-    <row r="35" spans="1:47">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -4526,7 +4526,7 @@
       <c r="AT35" s="1"/>
       <c r="AU35" s="1"/>
     </row>
-    <row r="36" spans="1:47">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -4585,7 +4585,7 @@
       <c r="AT36" s="1"/>
       <c r="AU36" s="1"/>
     </row>
-    <row r="37" spans="1:47">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -4640,7 +4640,7 @@
       <c r="AT37" s="1"/>
       <c r="AU37" s="1"/>
     </row>
-    <row r="38" spans="1:47">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -4693,7 +4693,7 @@
       <c r="AT38" s="1"/>
       <c r="AU38" s="1"/>
     </row>
-    <row r="39" spans="1:47">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -4742,7 +4742,7 @@
       <c r="AT39" s="1"/>
       <c r="AU39" s="1"/>
     </row>
-    <row r="40" spans="1:47">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -4791,7 +4791,7 @@
       <c r="AT40" s="1"/>
       <c r="AU40" s="1"/>
     </row>
-    <row r="41" spans="1:47">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4840,7 +4840,7 @@
       <c r="AT41" s="1"/>
       <c r="AU41" s="1"/>
     </row>
-    <row r="42" spans="1:47">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -4889,7 +4889,7 @@
       <c r="AT42" s="1"/>
       <c r="AU42" s="1"/>
     </row>
-    <row r="43" spans="1:47">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -4938,7 +4938,7 @@
       <c r="AT43" s="1"/>
       <c r="AU43" s="1"/>
     </row>
-    <row r="44" spans="1:47">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4987,7 +4987,7 @@
       <c r="AT44" s="1"/>
       <c r="AU44" s="1"/>
     </row>
-    <row r="45" spans="1:47">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5036,7 +5036,7 @@
       <c r="AT45" s="1"/>
       <c r="AU45" s="1"/>
     </row>
-    <row r="46" spans="1:47">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -5085,7 +5085,7 @@
       <c r="AT46" s="1"/>
       <c r="AU46" s="1"/>
     </row>
-    <row r="47" spans="1:47">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -5134,7 +5134,7 @@
       <c r="AT47" s="1"/>
       <c r="AU47" s="1"/>
     </row>
-    <row r="48" spans="1:47">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -5183,7 +5183,7 @@
       <c r="AT48" s="1"/>
       <c r="AU48" s="1"/>
     </row>
-    <row r="49" spans="1:47">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -5232,7 +5232,7 @@
       <c r="AT49" s="1"/>
       <c r="AU49" s="1"/>
     </row>
-    <row r="50" spans="1:47">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -5281,7 +5281,7 @@
       <c r="AT50" s="1"/>
       <c r="AU50" s="1"/>
     </row>
-    <row r="51" spans="1:47">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -5330,7 +5330,7 @@
       <c r="AT51" s="1"/>
       <c r="AU51" s="1"/>
     </row>
-    <row r="52" spans="1:47">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -5379,7 +5379,7 @@
       <c r="AT52" s="1"/>
       <c r="AU52" s="1"/>
     </row>
-    <row r="53" spans="1:47">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -5428,7 +5428,7 @@
       <c r="AT53" s="1"/>
       <c r="AU53" s="1"/>
     </row>
-    <row r="54" spans="1:47">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -5477,7 +5477,7 @@
       <c r="AT54" s="1"/>
       <c r="AU54" s="1"/>
     </row>
-    <row r="55" spans="1:47">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -5526,7 +5526,7 @@
       <c r="AT55" s="1"/>
       <c r="AU55" s="1"/>
     </row>
-    <row r="56" spans="1:47">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -5575,7 +5575,7 @@
       <c r="AT56" s="1"/>
       <c r="AU56" s="1"/>
     </row>
-    <row r="57" spans="1:47">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -5624,7 +5624,7 @@
       <c r="AT57" s="1"/>
       <c r="AU57" s="1"/>
     </row>
-    <row r="58" spans="1:47">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -5673,7 +5673,7 @@
       <c r="AT58" s="1"/>
       <c r="AU58" s="1"/>
     </row>
-    <row r="59" spans="1:47">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -5722,7 +5722,7 @@
       <c r="AT59" s="1"/>
       <c r="AU59" s="1"/>
     </row>
-    <row r="60" spans="1:47">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -5771,7 +5771,7 @@
       <c r="AT60" s="1"/>
       <c r="AU60" s="1"/>
     </row>
-    <row r="61" spans="1:47">
+    <row r="61" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -5820,7 +5820,7 @@
       <c r="AT61" s="1"/>
       <c r="AU61" s="1"/>
     </row>
-    <row r="62" spans="1:47">
+    <row r="62" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -5869,7 +5869,7 @@
       <c r="AT62" s="1"/>
       <c r="AU62" s="1"/>
     </row>
-    <row r="63" spans="1:47">
+    <row r="63" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -5918,7 +5918,7 @@
       <c r="AT63" s="1"/>
       <c r="AU63" s="1"/>
     </row>
-    <row r="64" spans="1:47">
+    <row r="64" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -5967,7 +5967,7 @@
       <c r="AT64" s="1"/>
       <c r="AU64" s="1"/>
     </row>
-    <row r="65" spans="1:47">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -6016,7 +6016,7 @@
       <c r="AT65" s="1"/>
       <c r="AU65" s="1"/>
     </row>
-    <row r="66" spans="1:47">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -6065,7 +6065,7 @@
       <c r="AT66" s="1"/>
       <c r="AU66" s="1"/>
     </row>
-    <row r="67" spans="1:47">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -6114,7 +6114,7 @@
       <c r="AT67" s="1"/>
       <c r="AU67" s="1"/>
     </row>
-    <row r="68" spans="1:47">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -6163,7 +6163,7 @@
       <c r="AT68" s="1"/>
       <c r="AU68" s="1"/>
     </row>
-    <row r="69" spans="1:47">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -6212,7 +6212,7 @@
       <c r="AT69" s="1"/>
       <c r="AU69" s="1"/>
     </row>
-    <row r="70" spans="1:47">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -6261,7 +6261,7 @@
       <c r="AT70" s="1"/>
       <c r="AU70" s="1"/>
     </row>
-    <row r="71" spans="1:47">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -6310,7 +6310,7 @@
       <c r="AT71" s="1"/>
       <c r="AU71" s="1"/>
     </row>
-    <row r="72" spans="1:47">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -6359,7 +6359,7 @@
       <c r="AT72" s="1"/>
       <c r="AU72" s="1"/>
     </row>
-    <row r="73" spans="1:47">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -6408,7 +6408,7 @@
       <c r="AT73" s="1"/>
       <c r="AU73" s="1"/>
     </row>
-    <row r="74" spans="1:47">
+    <row r="74" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -6455,7 +6455,7 @@
       <c r="AR74" s="1"/>
       <c r="AS74" s="1"/>
     </row>
-    <row r="75" spans="1:47">
+    <row r="75" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -6502,7 +6502,7 @@
       <c r="AR75" s="1"/>
       <c r="AS75" s="1"/>
     </row>
-    <row r="76" spans="1:47">
+    <row r="76" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -6549,7 +6549,7 @@
       <c r="AR76" s="1"/>
       <c r="AS76" s="1"/>
     </row>
-    <row r="77" spans="1:47">
+    <row r="77" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -6596,7 +6596,7 @@
       <c r="AR77" s="1"/>
       <c r="AS77" s="1"/>
     </row>
-    <row r="78" spans="1:47">
+    <row r="78" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -6638,7 +6638,7 @@
       <c r="AM78" s="1"/>
       <c r="AN78" s="1"/>
     </row>
-    <row r="79" spans="1:47">
+    <row r="79" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -6680,7 +6680,7 @@
       <c r="AM79" s="1"/>
       <c r="AN79" s="1"/>
     </row>
-    <row r="80" spans="1:47">
+    <row r="80" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -6722,7 +6722,7 @@
       <c r="AM80" s="1"/>
       <c r="AN80" s="1"/>
     </row>
-    <row r="81" spans="1:40">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -6764,7 +6764,7 @@
       <c r="AM81" s="1"/>
       <c r="AN81" s="1"/>
     </row>
-    <row r="82" spans="1:40">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -6806,7 +6806,7 @@
       <c r="AM82" s="1"/>
       <c r="AN82" s="1"/>
     </row>
-    <row r="83" spans="1:40">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -6848,7 +6848,7 @@
       <c r="AM83" s="1"/>
       <c r="AN83" s="1"/>
     </row>
-    <row r="84" spans="1:40">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -6890,7 +6890,7 @@
       <c r="AM84" s="1"/>
       <c r="AN84" s="1"/>
     </row>
-    <row r="85" spans="1:40">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -6932,7 +6932,7 @@
       <c r="AM85" s="1"/>
       <c r="AN85" s="1"/>
     </row>
-    <row r="86" spans="1:40">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -6974,7 +6974,7 @@
       <c r="AM86" s="1"/>
       <c r="AN86" s="1"/>
     </row>
-    <row r="87" spans="1:40">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -7016,7 +7016,7 @@
       <c r="AM87" s="1"/>
       <c r="AN87" s="1"/>
     </row>
-    <row r="88" spans="1:40">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -7058,7 +7058,7 @@
       <c r="AM88" s="1"/>
       <c r="AN88" s="1"/>
     </row>
-    <row r="89" spans="1:40">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -7100,7 +7100,7 @@
       <c r="AM89" s="1"/>
       <c r="AN89" s="1"/>
     </row>
-    <row r="90" spans="1:40">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -7142,7 +7142,7 @@
       <c r="AM90" s="1"/>
       <c r="AN90" s="1"/>
     </row>
-    <row r="91" spans="1:40">
+    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -7184,7 +7184,7 @@
       <c r="AM91" s="1"/>
       <c r="AN91" s="1"/>
     </row>
-    <row r="92" spans="1:40">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -7226,7 +7226,7 @@
       <c r="AM92" s="1"/>
       <c r="AN92" s="1"/>
     </row>
-    <row r="93" spans="1:40">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -7268,7 +7268,7 @@
       <c r="AM93" s="1"/>
       <c r="AN93" s="1"/>
     </row>
-    <row r="94" spans="1:40">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -7310,7 +7310,7 @@
       <c r="AM94" s="1"/>
       <c r="AN94" s="1"/>
     </row>
-    <row r="95" spans="1:40">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -7352,7 +7352,7 @@
       <c r="AM95" s="1"/>
       <c r="AN95" s="1"/>
     </row>
-    <row r="96" spans="1:40">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -7394,7 +7394,7 @@
       <c r="AM96" s="1"/>
       <c r="AN96" s="1"/>
     </row>
-    <row r="97" spans="1:40">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -7436,7 +7436,7 @@
       <c r="AM97" s="1"/>
       <c r="AN97" s="1"/>
     </row>
-    <row r="98" spans="1:40">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -7478,7 +7478,7 @@
       <c r="AM98" s="1"/>
       <c r="AN98" s="1"/>
     </row>
-    <row r="99" spans="1:40">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -7520,7 +7520,7 @@
       <c r="AM99" s="1"/>
       <c r="AN99" s="1"/>
     </row>
-    <row r="100" spans="1:40">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -7562,7 +7562,7 @@
       <c r="AM100" s="1"/>
       <c r="AN100" s="1"/>
     </row>
-    <row r="101" spans="1:40">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -7604,7 +7604,7 @@
       <c r="AM101" s="1"/>
       <c r="AN101" s="1"/>
     </row>
-    <row r="102" spans="1:40">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -7646,7 +7646,7 @@
       <c r="AM102" s="1"/>
       <c r="AN102" s="1"/>
     </row>
-    <row r="103" spans="1:40">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -7688,7 +7688,7 @@
       <c r="AM103" s="1"/>
       <c r="AN103" s="1"/>
     </row>
-    <row r="104" spans="1:40">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -7730,7 +7730,7 @@
       <c r="AM104" s="1"/>
       <c r="AN104" s="1"/>
     </row>
-    <row r="105" spans="1:40">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -7772,7 +7772,7 @@
       <c r="AM105" s="1"/>
       <c r="AN105" s="1"/>
     </row>
-    <row r="106" spans="1:40">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -7814,7 +7814,7 @@
       <c r="AM106" s="1"/>
       <c r="AN106" s="1"/>
     </row>
-    <row r="107" spans="1:40">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -7856,7 +7856,7 @@
       <c r="AM107" s="1"/>
       <c r="AN107" s="1"/>
     </row>
-    <row r="108" spans="1:40">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -7898,7 +7898,7 @@
       <c r="AM108" s="1"/>
       <c r="AN108" s="1"/>
     </row>
-    <row r="109" spans="1:40">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -7940,7 +7940,7 @@
       <c r="AM109" s="1"/>
       <c r="AN109" s="1"/>
     </row>
-    <row r="110" spans="1:40">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -7982,7 +7982,7 @@
       <c r="AM110" s="1"/>
       <c r="AN110" s="1"/>
     </row>
-    <row r="111" spans="1:40">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -8024,7 +8024,7 @@
       <c r="AM111" s="1"/>
       <c r="AN111" s="1"/>
     </row>
-    <row r="112" spans="1:40">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -8066,7 +8066,7 @@
       <c r="AM112" s="1"/>
       <c r="AN112" s="1"/>
     </row>
-    <row r="113" spans="1:40">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>

</xml_diff>